<commit_message>
updates to sample regression tests and specs
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
-  <si>
-    <t>test name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Static Error?</t>
   </si>
@@ -119,7 +116,7 @@
     <t>1.4.2. Wrong function parameters/return value</t>
   </si>
   <si>
-    <t>1.5.1. Anonymous function cannot return a value; 4.2. Subtype relations: assignment; 2.9.2. Assignment: Invalid LHS</t>
+    <t>1.5.1. Anonymous function cannot return a value</t>
   </si>
   <si>
     <t>function_Typos.p</t>
@@ -131,7 +128,58 @@
     <t>Error messages and TODOs</t>
   </si>
   <si>
-    <t>1.1.2. Payload type: invalid type; event expects no payload</t>
+    <t xml:space="preserve"> 4.2. Subtype relations: assignment</t>
+  </si>
+  <si>
+    <t>2.9.2. Assignment: Invalid LHS</t>
+  </si>
+  <si>
+    <t>1.4.2. Return value has incorrect type (undeclared return type)</t>
+  </si>
+  <si>
+    <t>1.1.2. Payload type: invalid payload type: event expects no payload</t>
+  </si>
+  <si>
+    <t>D:\PLanguage\PLang\Doc\Samples\New\Neg\Old\</t>
+  </si>
+  <si>
+    <t>Actions_1.p</t>
+  </si>
+  <si>
+    <t>original test name</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>1.2.2. Real and model machines</t>
+  </si>
+  <si>
+    <t>2.2. Dynamic creation of machines using "new"</t>
+  </si>
+  <si>
+    <t>2.3. "raise" stmt</t>
+  </si>
+  <si>
+    <t>2.4. "send" stmt</t>
+  </si>
+  <si>
+    <t>2.8. Assertions</t>
+  </si>
+  <si>
+    <t>3.3.1. "payload" primitive expression</t>
+  </si>
+  <si>
+    <t>3.3.6. Cast operator "as"</t>
+  </si>
+  <si>
+    <t>4.3. Passing variables as payloads: variable of "ghost machine" type</t>
+  </si>
+  <si>
+    <t>1.8.2. Do declaration: action on named function</t>
+  </si>
+  <si>
+    <t>2.9.1. Assign on bool</t>
   </si>
 </sst>
 </file>
@@ -459,167 +507,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="61.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="56.85546875" customWidth="1"/>
+    <col min="6" max="6" width="104.28515625" customWidth="1"/>
     <col min="7" max="7" width="167.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated regression test tool and sample tests
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLanguage\PLang\Doc\TestDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLanguage\PLang1001\plang\Doc\TestDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -149,9 +149,6 @@
     <t>original test name</t>
   </si>
   <si>
-    <t>Integration</t>
-  </si>
-  <si>
     <t>1.2.2. Real and model machines</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>2.9.1. Assign on bool</t>
+  </si>
+  <si>
+    <t>Feature Integration</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -715,52 +715,52 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New title doc on regression testing and regression tests populated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Static Error?</t>
   </si>
@@ -140,15 +140,6 @@
     <t>1.1.2. Payload type: invalid payload type: event expects no payload</t>
   </si>
   <si>
-    <t>D:\PLanguage\PLang\Doc\Samples\New\Neg\Old\</t>
-  </si>
-  <si>
-    <t>Actions_1.p</t>
-  </si>
-  <si>
-    <t>original test name</t>
-  </si>
-  <si>
     <t>1.2.2. Real and model machines</t>
   </si>
   <si>
@@ -180,6 +171,21 @@
   </si>
   <si>
     <t>Feature Integration</t>
+  </si>
+  <si>
+    <t>Integration\DynamicError\Actions_1\Actions_1.p</t>
+  </si>
+  <si>
+    <t>test location</t>
+  </si>
+  <si>
+    <t>Formerly: D:\PLanguage\PLang\Doc\Samples\New\Neg\Old\</t>
+  </si>
+  <si>
+    <t>Formerly: D:\PLanguage\PLang\Doc\Samples\New</t>
+  </si>
+  <si>
+    <t>yellow rows: populated to RegressionTests</t>
   </si>
 </sst>
 </file>
@@ -203,12 +209,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,10 +235,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,12 +523,12 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="61.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="5" width="18.7109375" customWidth="1"/>
@@ -525,7 +538,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>28</v>
@@ -546,9 +559,14 @@
         <v>33</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -571,20 +589,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -695,72 +713,72 @@
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new tests added to regression test suite
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>Static Error?</t>
   </si>
@@ -186,13 +186,68 @@
   </si>
   <si>
     <t>yellow rows: populated to RegressionTests</t>
+  </si>
+  <si>
+    <t>Actions_3.p</t>
+  </si>
+  <si>
+    <t>Based on Actions_1.p, but with push and pop added</t>
+  </si>
+  <si>
+    <t>1.7.2. Transition Declaration: push transition</t>
+  </si>
+  <si>
+    <t>Actions_4.p</t>
+  </si>
+  <si>
+    <t>Similar to Actions_3.p, but with two asserts in a row: the 1st assert passes, the 2nd assert fails</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.8. Assertions: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>two asserts in a row</t>
+    </r>
+  </si>
+  <si>
+    <t>Actions_5.p</t>
+  </si>
+  <si>
+    <t>BangaloreToRedmond</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Call_Exit_1</t>
+  </si>
+  <si>
+    <t>Call_Exit_2</t>
+  </si>
+  <si>
+    <t>Call_Exit_3</t>
+  </si>
+  <si>
+    <t>CallStatement_1</t>
+  </si>
+  <si>
+    <t>Identical to BangaloreToRedmond, but using "with": on default goto TakeBus with { RemoteCheckIn = true; };</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +258,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -235,11 +298,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +782,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
@@ -736,49 +802,309 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new tests added to the regression suite
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="83">
   <si>
     <t>Static Error?</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Dynamic Error?</t>
   </si>
   <si>
-    <t>anonFunction.p</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>Other features tested</t>
   </si>
   <si>
-    <t>Duplicates.p</t>
-  </si>
-  <si>
     <t>anonfunction.p (13, 3): transition to an undefined state</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>comment in the test</t>
   </si>
   <si>
-    <t>Elevator.p</t>
-  </si>
-  <si>
     <t>Interaction</t>
   </si>
   <si>
@@ -77,12 +68,6 @@
     <t>2.12. ITE statements: if ($) in non- model machine and function</t>
   </si>
   <si>
-    <t>entryExit_1.p</t>
-  </si>
-  <si>
-    <t>entryExit_2.p</t>
-  </si>
-  <si>
     <t>1.6.2. Undefined function as entry/exit action</t>
   </si>
   <si>
@@ -95,18 +80,12 @@
     <t>1.8.1.Action on default (no error)</t>
   </si>
   <si>
-    <t>fields.p</t>
-  </si>
-  <si>
     <t>3.3.4.2. Bad field name</t>
   </si>
   <si>
     <t>4.2. Subtype relations: assignment</t>
   </si>
   <si>
-    <t>function.p</t>
-  </si>
-  <si>
     <t xml:space="preserve">P feature tested </t>
   </si>
   <si>
@@ -116,9 +95,6 @@
     <t>1.5.1. Anonymous function cannot return a value</t>
   </si>
   <si>
-    <t>function_Typos.p</t>
-  </si>
-  <si>
     <t>4.1.1. Tuples: duplicate names (in seq decl, in func decl, in payload)</t>
   </si>
   <si>
@@ -134,6 +110,9 @@
     <t>1.1.2. Payload type: invalid payload type: event expects no payload</t>
   </si>
   <si>
+    <t>Actions_1.p</t>
+  </si>
+  <si>
     <t>1.2.2. Real and model machines</t>
   </si>
   <si>
@@ -158,18 +137,12 @@
     <t>4.3. Passing variables as payloads: variable of "ghost machine" type</t>
   </si>
   <si>
-    <t>1.8.2. Do declaration: action on named function</t>
-  </si>
-  <si>
     <t>2.9.1. Assign on bool</t>
   </si>
   <si>
     <t>Feature Integration</t>
   </si>
   <si>
-    <t>Integration\DynamicError\Actions_1\Actions_1.p</t>
-  </si>
-  <si>
     <t>test location</t>
   </si>
   <si>
@@ -182,16 +155,7 @@
     <t>yellow rows: populated to RegressionTests</t>
   </si>
   <si>
-    <t>Actions_3.p</t>
-  </si>
-  <si>
     <t>Based on Actions_1.p, but with push and pop added</t>
-  </si>
-  <si>
-    <t>1.7.2. Transition Declaration: push transition</t>
-  </si>
-  <si>
-    <t>Actions_4.p</t>
   </si>
   <si>
     <t>Similar to Actions_3.p, but with two asserts in a row: the 1st assert passes, the 2nd assert fails</t>
@@ -213,9 +177,6 @@
     </r>
   </si>
   <si>
-    <t>Actions_5.p</t>
-  </si>
-  <si>
     <t>BangaloreToRedmond</t>
   </si>
   <si>
@@ -228,9 +189,6 @@
     <t>Call_Exit_2</t>
   </si>
   <si>
-    <t>Call_Exit_3</t>
-  </si>
-  <si>
     <t>CallStatement_1</t>
   </si>
   <si>
@@ -241,6 +199,93 @@
   </si>
   <si>
     <t>1.4.3. Return value has incorrect type (undeclared return type)</t>
+  </si>
+  <si>
+    <t>1.8.2.1. Do declaration: action on named function</t>
+  </si>
+  <si>
+    <t>Based on Actions_1.p, but zing passes: there's push, but no pop, so asserts are never reached</t>
+  </si>
+  <si>
+    <t>1.7.2.2. Transition declaration: push transition, no pop</t>
+  </si>
+  <si>
+    <t>1.7.2.1. Transition Declaration: push transition</t>
+  </si>
+  <si>
+    <t>TODO 1.7.2.2</t>
+  </si>
+  <si>
+    <t>AlonBug</t>
+  </si>
+  <si>
+    <t>BangaloreToRedmond_Liveness</t>
+  </si>
+  <si>
+    <t>MaxInstances_2</t>
+  </si>
+  <si>
+    <t>PingPong</t>
+  </si>
+  <si>
+    <t>Actions_6</t>
+  </si>
+  <si>
+    <t>Actions_5</t>
+  </si>
+  <si>
+    <t>Actions_4</t>
+  </si>
+  <si>
+    <t>Actions_3</t>
+  </si>
+  <si>
+    <t>Actions_2</t>
+  </si>
+  <si>
+    <t>anonFunction</t>
+  </si>
+  <si>
+    <t>Duplicates</t>
+  </si>
+  <si>
+    <t>Elevator</t>
+  </si>
+  <si>
+    <t>entryExit_1</t>
+  </si>
+  <si>
+    <t>entryExit_2</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>function_Typos</t>
+  </si>
+  <si>
+    <t>PingPongDingDong</t>
+  </si>
+  <si>
+    <t>PingPongWithCall</t>
+  </si>
+  <si>
+    <t>TODO: what is "with" in transition? can it be used with any transition?</t>
+  </si>
+  <si>
+    <t>1.7.2.3. Pairwise push/pop in a loop</t>
+  </si>
+  <si>
+    <t>3.3.3.1. Binary Add</t>
+  </si>
+  <si>
+    <t>2.9.1. Assign on int</t>
+  </si>
+  <si>
+    <t>2.8. two asserts in a row with complimentary conditions</t>
   </si>
 </sst>
 </file>
@@ -586,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,10 +649,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -616,23 +661,23 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -640,471 +685,638 @@
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="4" t="s">
-        <v>36</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
-        <v>44</v>
+      <c r="F30" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F41" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>60</v>
+        <v>78</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F56" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test docs updated according to rules and errors in P.4ml (in progress)
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="171">
   <si>
     <t>Static Error?</t>
   </si>
@@ -507,9 +507,6 @@
     <t>"No Main Machine"; "no start state in machine"</t>
   </si>
   <si>
-    <t>"no start state in machine"</t>
-  </si>
-  <si>
     <t>"transition to an undefined state"</t>
   </si>
   <si>
@@ -522,13 +519,25 @@
     <t xml:space="preserve">1.6.2. Undefined function for exit </t>
   </si>
   <si>
-    <t>"model functions can be declared only in real machines"; "Nondeterminitistic choice can be used only in model machine and model functions" (both cases tested)</t>
-  </si>
-  <si>
-    <t>"model functions can be declared only in real machines"; "default transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"No Main Machine"; "no start state in machine", "function cannot take arguments" (for entry and exit); “Bad field name" </t>
+    <t>"model functions can be declared only in real machines"; "Nondeterminitistic choice can be used only in model machine and model functions" (both cases tested); ""if (...)" expects a boolean value";</t>
+  </si>
+  <si>
+    <t>"argument 1 of "raise" expects an event value"; "argument 2 of "send" expects an event value"</t>
+  </si>
+  <si>
+    <t>"no start state in machine"; "return value has incorrect type"; "invalid payload type in send"</t>
+  </si>
+  <si>
+    <t>"function requires arguments"; "return value has incorrect type"; "function must return a value"; "anonymous function cannot return a value"; "invalid assignment. right hand side is not a subtype of left hand side"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"invalid payload type in raise"; "invalid payload type in send"; "invalid assignment. right hand side is not a subtype of left hand side"; </t>
+  </si>
+  <si>
+    <t>"model functions can be declared only in real machines"; "default transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side";</t>
+  </si>
+  <si>
+    <t>"No Main Machine"; "no start state in machine", "function cannot take arguments" (for entry and exit); “Bad field name"; "Operator expected first argument to be an integer value"; "invalid assignment. right hand side is not a subtype of left hand side";</t>
   </si>
 </sst>
 </file>
@@ -876,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -946,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>5</v>
@@ -1026,7 +1035,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,10 +1049,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>11</v>
@@ -1063,7 +1072,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1079,6 +1088,9 @@
       <c r="F15" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" s="1" t="s">
@@ -1104,7 +1116,7 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1157,7 +1169,7 @@
         <v>83</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1252,6 +1264,9 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1280,6 +1295,9 @@
       <c r="F30" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
@@ -1310,7 +1328,7 @@
         <v>140</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tests and test docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
   </bookViews>
   <sheets>
-    <sheet name="SamplesNewTests" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
+    <sheet name="RegressionTestsLong" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
   <si>
     <t>Static Error?</t>
   </si>
@@ -396,9 +396,6 @@
     <t>Push_Pop_2</t>
   </si>
   <si>
-    <t>Part of RegressionTestsLong: Zing takes about 5 min to come up with the "pass" result</t>
-  </si>
-  <si>
     <t>1.2.4.2. Monitors: not allowed: new, send, push, pop, model functions, defer, default trans</t>
   </si>
   <si>
@@ -538,6 +535,39 @@
   </si>
   <si>
     <t>"No Main Machine"; "no start state in machine", "function cannot take arguments" (for entry and exit); “Bad field name"; "Operator expected first argument to be an integer value"; "invalid assignment. right hand side is not a subtype of left hand side";</t>
+  </si>
+  <si>
+    <t>"invalid assignment. right hand side is not a subtype of left hand side"</t>
+  </si>
+  <si>
+    <t>nmdType</t>
+  </si>
+  <si>
+    <t>2.9.1. 2.9.1. Assignment: types of LHS and RHS: wrong names in named tuples</t>
+  </si>
+  <si>
+    <t>Formerly: D:\PLanguage\PLang\Doc\Samples\New\Examples</t>
+  </si>
+  <si>
+    <t>boundedasync</t>
+  </si>
+  <si>
+    <t>TODO: what is it testing?</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Also, included into RegressionTestsLong: Zing takes about 5 min to come up with the "pass" result</t>
+  </si>
+  <si>
+    <t>Also, included into RegressionTests as pure static check; Zing takes about 5 min to come up with the "pass" result</t>
+  </si>
+  <si>
+    <t>Integration (static check only)</t>
+  </si>
+  <si>
+    <t>Feature Integration (static check only)</t>
   </si>
 </sst>
 </file>
@@ -883,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,10 +952,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -955,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>5</v>
@@ -975,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>73</v>
@@ -1035,7 +1065,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1049,10 +1079,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>11</v>
@@ -1072,7 +1102,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1089,7 +1119,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1116,7 +1146,7 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1152,7 +1182,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1160,7 +1190,7 @@
         <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
@@ -1169,7 +1199,7 @@
         <v>83</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1182,7 +1212,7 @@
         <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -1194,7 +1224,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1214,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,13 +1255,13 @@
         <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1239,7 +1269,7 @@
         <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
@@ -1248,10 +1278,10 @@
         <v>81</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1259,21 +1289,21 @@
         <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>105</v>
@@ -1284,96 +1314,96 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F33" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F35" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F36" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F38" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
@@ -1387,177 +1417,125 @@
     </row>
     <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>34</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F45" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F47" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F48" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F49" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F50" s="1" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F51" s="1" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F52" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F53" s="1" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F54" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F55" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F56" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F60" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F61" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -1565,21 +1543,37 @@
       <c r="D63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>109</v>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F64" s="1" t="s">
-        <v>108</v>
+      <c r="A64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>119</v>
+        <v>48</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
@@ -1587,19 +1581,15 @@
       <c r="D65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>47</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
@@ -1608,139 +1598,131 @@
         <v>2</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F68" s="1" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F69" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F74" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F70" s="1" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F75" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+    <row r="78" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F78" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
@@ -1750,20 +1732,25 @@
       </c>
       <c r="E79" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>2</v>
@@ -1771,13 +1758,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>2</v>
@@ -1785,7 +1772,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>32</v>
@@ -1800,66 +1787,156 @@
         <v>2</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F83" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>153</v>
+      <c r="C87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>8</v>
+      <c r="C93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1870,14 +1947,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD28"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="52.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test doc and testconfig.txt updates
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
-    <sheet name="RegressionTestsLong" sheetId="2" r:id="rId2"/>
+    <sheet name="SamplesProtocols" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="179">
   <si>
     <t>Static Error?</t>
   </si>
@@ -165,9 +165,6 @@
     <t>PingPong</t>
   </si>
   <si>
-    <t>Actions_6</t>
-  </si>
-  <si>
     <t>Actions_5</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
     <t>AlonBug_fails</t>
   </si>
   <si>
-    <t>Feature Integration: Feature Integration: 2.1.2. Deferred-by-default semantics of push statement</t>
-  </si>
-  <si>
     <t>Feature Integration: 2.1.2. Deferred-by-default semantics of push statement</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
     <t>1.7.2.3. Inheritance of actions but not of transitions</t>
   </si>
   <si>
-    <t>Feature Integration: 1.7.2.3. Payload with push transitions</t>
-  </si>
-  <si>
     <t>1.9/1.10 Assert/Assume Max Instances of an event (syntax)</t>
   </si>
   <si>
@@ -405,18 +396,12 @@
     <t>Monitor added to PingPong test</t>
   </si>
   <si>
-    <t>Feature Integration: (TODO: which features?)</t>
-  </si>
-  <si>
     <t>2.4. Send statement: type checking</t>
   </si>
   <si>
     <t>TokenRing</t>
   </si>
   <si>
-    <t>Integration: 1.10 Attempting to enqueue event more than max instance of 1</t>
-  </si>
-  <si>
     <t>TokenRing_Typos</t>
   </si>
   <si>
@@ -462,18 +447,12 @@
     <t>two-phase-commit</t>
   </si>
   <si>
-    <t>Integration</t>
-  </si>
-  <si>
     <t>Zing did not finish in 19 hours; TODO: discuss with Shaz</t>
   </si>
   <si>
     <t>zing hasn't finished in 23 hours; TODO: discuss with Shaz</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>1.4.4. Data impure functions</t>
   </si>
   <si>
@@ -552,9 +531,6 @@
     <t>boundedasync</t>
   </si>
   <si>
-    <t>TODO: what is it testing?</t>
-  </si>
-  <si>
     <t>German</t>
   </si>
   <si>
@@ -564,10 +540,28 @@
     <t>Also, included into RegressionTests as pure static check; Zing takes about 5 min to come up with the "pass" result</t>
   </si>
   <si>
-    <t>Integration (static check only)</t>
-  </si>
-  <si>
-    <t>Feature Integration (static check only)</t>
+    <t>Zing takes too long</t>
+  </si>
+  <si>
+    <t>TODO: zing hasn't finished in ~20 hours</t>
+  </si>
+  <si>
+    <t>function_any</t>
+  </si>
+  <si>
+    <t>1.7.2.3. Payload with push transitions</t>
+  </si>
+  <si>
+    <t>Feature Integration: protocol sample, syntax only</t>
+  </si>
+  <si>
+    <t>1.10 Attempting to enqueue event more than max instance of 1</t>
+  </si>
+  <si>
+    <t>Integration: Attempting to enqueue event more than max instance of 1</t>
+  </si>
+  <si>
+    <t>Feature Integration: protocol sample</t>
   </si>
 </sst>
 </file>
@@ -915,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,10 +946,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -973,7 +967,7 @@
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>39</v>
@@ -985,7 +979,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>5</v>
@@ -993,7 +987,7 @@
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
@@ -1005,15 +999,15 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>32</v>
@@ -1028,35 +1022,35 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -1065,12 +1059,12 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1079,10 +1073,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>11</v>
@@ -1090,7 +1084,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1102,12 +1096,12 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1119,7 +1113,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1134,7 +1128,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1146,7 +1140,7 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1156,10 +1150,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
@@ -1173,33 +1167,33 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1209,10 +1203,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -1224,12 +1218,12 @@
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>32</v>
@@ -1244,166 +1238,166 @@
         <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F32" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F33" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F35" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F36" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F38" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>145</v>
+        <v>175</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
@@ -1417,35 +1411,41 @@
     </row>
     <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>145</v>
+        <v>175</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1458,7 +1458,7 @@
         <v>22</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>8</v>
@@ -1472,12 +1472,12 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F50" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F51" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F53" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1532,10 +1532,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -1546,15 +1546,15 @@
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>8</v>
@@ -1565,15 +1565,15 @@
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
@@ -1598,15 +1598,15 @@
         <v>2</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>99</v>
+        <v>174</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
@@ -1620,7 +1620,7 @@
         <v>37</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>8</v>
@@ -1629,17 +1629,17 @@
         <v>2</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F69" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>32</v>
@@ -1651,7 +1651,7 @@
         <v>2</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>38</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>32</v>
@@ -1671,15 +1671,15 @@
         <v>2</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>32</v>
@@ -1691,38 +1691,38 @@
         <v>2</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F73" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F74" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F75" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
@@ -1736,7 +1736,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
         <v>42</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
@@ -1758,10 +1758,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -1775,7 +1775,7 @@
         <v>43</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
@@ -1787,15 +1787,15 @@
         <v>2</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F83" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -1803,7 +1803,7 @@
         <v>44</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>8</v>
@@ -1817,16 +1817,16 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>2</v>
@@ -1834,13 +1834,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>2</v>
@@ -1851,7 +1851,7 @@
         <v>45</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>8</v>
@@ -1863,15 +1863,15 @@
         <v>2</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>8</v>
@@ -1883,60 +1883,63 @@
         <v>2</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D89" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="H89" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1947,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,15 +1986,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -2006,7 +2009,17 @@
         <v>2</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new tests added; test docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="182">
   <si>
     <t>Static Error?</t>
   </si>
@@ -562,6 +562,15 @@
   </si>
   <si>
     <t>Feature Integration: protocol sample</t>
+  </si>
+  <si>
+    <t>LinearTopology_5</t>
+  </si>
+  <si>
+    <t>openwsn1</t>
+  </si>
+  <si>
+    <t>Formerly: D:\PLanguage\PLang\Doc\Samples\New\PayloadTypeInference</t>
   </si>
 </sst>
 </file>
@@ -907,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,6 +1434,9 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>80</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -1442,227 +1454,148 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>80</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F50" s="1" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F51" s="1" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F52" s="1" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F53" s="1" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F54" s="1" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F55" s="1" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F56" s="1" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F57" s="1" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F65" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F58" s="1" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F66" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F59" s="1" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F67" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F60" s="1" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F68" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F61" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F69" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>8</v>
@@ -1670,188 +1603,186 @@
       <c r="D71" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
       <c r="H71" s="1" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F77" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F73" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F74" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F75" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>63</v>
+      <c r="C78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="H79" s="1" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>2</v>
+      <c r="F81" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F82" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F83" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>2</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>8</v>
@@ -1862,16 +1793,18 @@
       <c r="E87" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>110</v>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>8</v>
@@ -1881,48 +1814,79 @@
       </c>
       <c r="E88" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>145</v>
+      <c r="C90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F91" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>2</v>
@@ -1930,15 +1894,111 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G94" s="1" t="s">
+      <c r="C102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G102" s="1" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Regression tool updated with printing summary results; tests added, docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="195">
   <si>
     <t>Static Error?</t>
   </si>
@@ -571,6 +571,45 @@
   </si>
   <si>
     <t>Formerly: D:\PLanguage\PLang\Doc\Samples\New\PayloadTypeInference</t>
+  </si>
+  <si>
+    <t>payloadActions</t>
+  </si>
+  <si>
+    <t>payloadActionsFuns</t>
+  </si>
+  <si>
+    <t>payloadEntry</t>
+  </si>
+  <si>
+    <t>payloadEntry_1</t>
+  </si>
+  <si>
+    <t>payloadEntryFuns</t>
+  </si>
+  <si>
+    <t>payloadExit</t>
+  </si>
+  <si>
+    <t>payloadExitFuns</t>
+  </si>
+  <si>
+    <t>payloadStartState</t>
+  </si>
+  <si>
+    <t>payloadTransitions</t>
+  </si>
+  <si>
+    <t>payloadTransitionsFuns</t>
+  </si>
+  <si>
+    <t>4.3. Paylod type inference</t>
+  </si>
+  <si>
+    <t>payloads</t>
+  </si>
+  <si>
+    <t>"invalid payload type in send"; "invalid payload type in send (cannot send null value)"; "invalid payload type in raise"; "argument 1 of "send" expects a machine value"; "argument 2 of "send" expects a machine value"</t>
   </si>
 </sst>
 </file>
@@ -916,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,201 +1547,237 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F58" s="1" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F59" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F61" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F62" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F63" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F64" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F65" s="1" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F66" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F67" s="1" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F68" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F69" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F70" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F71" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F72" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F74" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F75" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="1" t="s">
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F77" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>8</v>
@@ -1710,19 +1785,18 @@
       <c r="D78" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
       <c r="H78" s="1" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
@@ -1730,19 +1804,15 @@
       <c r="D79" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
@@ -1751,184 +1821,181 @@
         <v>2</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F81" s="1" t="s">
-        <v>60</v>
+      <c r="A81" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F82" s="1" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F83" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F87" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F88" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F89" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+    <row r="92" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F91" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>178</v>
+        <v>104</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>110</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>178</v>
@@ -1943,40 +2010,71 @@
         <v>2</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F97" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
-        <v>145</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>8</v>
@@ -1986,19 +2084,84 @@
       </c>
       <c r="E101" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G102" s="1" t="s">
+      <c r="C108" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test samples and docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="211">
   <si>
     <t>Static Error?</t>
   </si>
@@ -540,15 +540,6 @@
     <t>Also, included into RegressionTests as pure static check; Zing takes about 5 min to come up with the "pass" result</t>
   </si>
   <si>
-    <t>Zing takes too long</t>
-  </si>
-  <si>
-    <t>TODO: zing hasn't finished in ~20 hours</t>
-  </si>
-  <si>
-    <t>function_any</t>
-  </si>
-  <si>
     <t>1.7.2.3. Payload with push transitions</t>
   </si>
   <si>
@@ -610,6 +601,63 @@
   </si>
   <si>
     <t>"invalid payload type in send"; "invalid payload type in send (cannot send null value)"; "invalid payload type in raise"; "argument 1 of "send" expects a machine value"; "argument 2 of "send" expects a machine value"</t>
+  </si>
+  <si>
+    <t>Zing stats when no limits</t>
+  </si>
+  <si>
+    <t>states/trans/depth, min</t>
+  </si>
+  <si>
+    <t>26764/75314/34, 5-6 min</t>
+  </si>
+  <si>
+    <t>Also, included into RegressionTests as pure static check</t>
+  </si>
+  <si>
+    <t>delayc</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Zing takes &gt;40 min for delayc values &gt; 1 TODO: try depth bounding ot other dlls for delay bounding</t>
+  </si>
+  <si>
+    <t>total transitions</t>
+  </si>
+  <si>
+    <t>distinct states</t>
+  </si>
+  <si>
+    <t>max depth (steps)</t>
+  </si>
+  <si>
+    <t>time (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-3</t>
+  </si>
+  <si>
+    <t>Zing takes &gt;6 min for delayc values &gt; 2 TODO: try depth bounding ot other dlls for delay bounding</t>
+  </si>
+  <si>
+    <t>functionAny (formerly function_any)</t>
+  </si>
+  <si>
+    <t>Zing params: -delayc:4, -sched:RunToCompletionDBSched.dll</t>
+  </si>
+  <si>
+    <t>Zing params: -delayc:2, -sched:RunToCompletionDBSched.dll</t>
+  </si>
+  <si>
+    <t>Zing params: -delayc:1, -sched:RunToCompletionDBSched.dll</t>
+  </si>
+  <si>
+    <t>Zing takes &gt; 15min even with  -delayc:1, -sched:RunToCompletionDBSched.dll, -bc:1</t>
   </si>
 </sst>
 </file>
@@ -667,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -675,6 +723,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1304,7 @@
         <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -1311,7 +1361,7 @@
         <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
@@ -1342,7 +1392,7 @@
         <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>102</v>
@@ -1351,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1428,7 +1478,7 @@
         <v>139</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1467,7 +1517,7 @@
         <v>167</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
@@ -1476,10 +1526,10 @@
         <v>8</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1487,7 +1537,7 @@
         <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
@@ -1496,18 +1546,18 @@
         <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
@@ -1516,18 +1566,18 @@
         <v>8</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
@@ -1539,20 +1589,20 @@
         <v>80</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>2</v>
@@ -1560,10 +1610,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>2</v>
@@ -1571,10 +1621,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>2</v>
@@ -1582,10 +1632,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>2</v>
@@ -1593,10 +1643,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>2</v>
@@ -1604,10 +1654,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>2</v>
@@ -1615,10 +1665,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>2</v>
@@ -1626,24 +1676,24 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>2</v>
@@ -1651,10 +1701,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>2</v>
@@ -1662,10 +1712,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>2</v>
@@ -1826,15 +1876,18 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1843,7 +1896,7 @@
         <v>37</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
@@ -1998,7 +2051,7 @@
         <v>43</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>8</v>
@@ -2074,7 +2127,7 @@
         <v>45</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>8</v>
@@ -2094,7 +2147,7 @@
         <v>58</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>8</v>
@@ -2114,7 +2167,7 @@
         <v>59</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>8</v>
@@ -2173,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N3" sqref="N3:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,12 +2237,19 @@
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="8" width="52.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" customWidth="1"/>
+    <col min="15" max="15" width="83.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2214,38 +2274,438 @@
       <c r="H1" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5">
+        <v>17934</v>
+      </c>
+      <c r="K4" s="5">
+        <v>75212</v>
+      </c>
+      <c r="L4" s="5">
+        <v>72</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="8">
+        <v>30114</v>
+      </c>
+      <c r="K5" s="8">
+        <v>81109</v>
+      </c>
+      <c r="L5" s="8">
+        <v>254</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>168</v>
       </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>320804</v>
+      </c>
+      <c r="K6" s="8">
+        <v>551168</v>
+      </c>
+      <c r="L6" s="8">
+        <v>123</v>
+      </c>
+      <c r="M6" s="8">
+        <v>4</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>195</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>235817</v>
+      </c>
+      <c r="K7" s="8">
+        <v>376901</v>
+      </c>
+      <c r="L7" s="8">
+        <v>143</v>
+      </c>
+      <c r="M7" s="8">
+        <v>5</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>195</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
regression folder tree changed (separate folders for Pc, Zinger, Runtime for each test); testP tool and docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="217">
   <si>
     <t>Static Error?</t>
   </si>
@@ -658,6 +658,24 @@
   </si>
   <si>
     <t>Zing takes &gt; 15min even with  -delayc:1, -sched:RunToCompletionDBSched.dll, -bc:1</t>
+  </si>
+  <si>
+    <t>Max_Instances_4</t>
+  </si>
+  <si>
+    <t>Feature Integration ???</t>
+  </si>
+  <si>
+    <t>two-phase-commit_1</t>
+  </si>
+  <si>
+    <t>Multi_Paxos_3</t>
+  </si>
+  <si>
+    <t>Multi_Paxos_4</t>
+  </si>
+  <si>
+    <t>Also added as syntactic check only</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,27 +2142,15 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>175</v>
@@ -2159,12 +2165,12 @@
         <v>2</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>175</v>
@@ -2173,49 +2179,123 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F103" s="1" t="s">
+      <c r="F104" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H103" s="1" t="s">
+      <c r="H104" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G108" s="1" t="s">
+      <c r="C109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semantics regression tests added; docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
-    <sheet name="SamplesProtocols" sheetId="2" r:id="rId2"/>
+    <sheet name="NewSemTests" sheetId="3" r:id="rId2"/>
+    <sheet name="SamplesProtocols" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="257">
   <si>
     <t>Static Error?</t>
   </si>
@@ -126,9 +127,6 @@
     <t>Feature Integration</t>
   </si>
   <si>
-    <t>test location</t>
-  </si>
-  <si>
     <t>Formerly: D:\PLanguage\PLang\Doc\Samples\New\Neg\Old\</t>
   </si>
   <si>
@@ -279,9 +277,6 @@
     <t xml:space="preserve">Feature Integration: 1.6.5.2. basic semantics of actions </t>
   </si>
   <si>
-    <t>1.7.2.4. Goto transition</t>
-  </si>
-  <si>
     <t>Based on Actions_1.p, but zing passes: shows difference between inheritance when using "do" and "goto" after "push"</t>
   </si>
   <si>
@@ -294,9 +289,6 @@
     <t>2.1. Push statement</t>
   </si>
   <si>
-    <t>1.7.2. "push" transition</t>
-  </si>
-  <si>
     <t>PushStatement_1 (formerly CallStatement_1)</t>
   </si>
   <si>
@@ -682,6 +674,129 @@
   </si>
   <si>
     <t xml:space="preserve"> Zing params: -delayc:2, -sched:RunToCompletionDBSched.dll; for delayc values &gt; 2, Zing takes more than 10 min</t>
+  </si>
+  <si>
+    <t>RaiseInExitFun</t>
+  </si>
+  <si>
+    <t>Combined: Control Impurity: error when "raise" in exit function</t>
+  </si>
+  <si>
+    <t>"function may cause a change in current state; this is not allowed here"</t>
+  </si>
+  <si>
+    <t>PopInExitFun</t>
+  </si>
+  <si>
+    <t>Combined: Control Impurity: error when "push" in exit function</t>
+  </si>
+  <si>
+    <t>PushInExitFun</t>
+  </si>
+  <si>
+    <t>Combined: Control Impurity: error when "pop" in exit function</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test </t>
+  </si>
+  <si>
+    <t>2.3.1. “raise” in entry handled in the same state; 2.4.1. “send” in entry handled in the same state</t>
+  </si>
+  <si>
+    <t>"send" after "raise" in entry actions is a "no action"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.4.1. “send” in entry handled in the same state</t>
+  </si>
+  <si>
+    <t>1.7.2.2. Goto transition</t>
+  </si>
+  <si>
+    <t>1.7.2.3. "push" transition</t>
+  </si>
+  <si>
+    <t>1.7.2.2. Simple semantics of "goto" transition</t>
+  </si>
+  <si>
+    <t>this test is a pair to SendInExitHandledEvent.p</t>
+  </si>
+  <si>
+    <t>this test is a pair to SendInExitUnhandledEvent.p</t>
+  </si>
+  <si>
+    <t>"Unhandled event exception by machine Real1-0"</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_1\SendRaiseInEntry.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_2\RaiseSendInEntry.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_3\SendInEntry.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_4\SendInExitNotExecuted.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_5\SendInExitUnhandledEvent.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_6\SendInExitHandledEvent.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_7\SendInExitUnhandledHalt.p</t>
+  </si>
+  <si>
+    <t>Compare to SEM_OneMachine_5\SendInExitUnhandledEvent.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine,  "send" to itself and "raise" in entry actions</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, 'raise" and "send" to itself in entry actions</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "send" to itself in entry actions</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine,"send" to itself in exit not executed</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine,  "send" to itself in exit function</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "send" to itself in exit function</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_8\GotoToItself.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "goto" to the same state; "send" in entry and exit</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_9\PushItself.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "push" and "goto" to the same state; "send" in entry and exit</t>
+  </si>
+  <si>
+    <t>1.1.1.2. Assert Max Instances of an event</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_10\Push.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "push", "send" in entry and exit</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_11\PushImplicitPop.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "push" with implicit "pop"</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:XFD110"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1165,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>223</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -1068,20 +1183,20 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -1089,10 +1204,10 @@
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
@@ -1101,7 +1216,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>5</v>
@@ -1109,7 +1224,7 @@
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
@@ -1121,15 +1236,15 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>32</v>
@@ -1144,35 +1259,35 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -1181,12 +1296,12 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1195,10 +1310,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>11</v>
@@ -1206,7 +1321,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1218,12 +1333,12 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1235,7 +1350,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1250,7 +1365,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1262,20 +1377,20 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
@@ -1289,33 +1404,33 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1325,10 +1440,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -1340,12 +1455,12 @@
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>32</v>
@@ -1360,149 +1475,149 @@
         <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F32" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F33" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F35" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F36" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F38" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1514,15 +1629,15 @@
         <v>2</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
@@ -1536,15 +1651,15 @@
     </row>
     <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
@@ -1556,16 +1671,16 @@
         <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1576,15 +1691,15 @@
         <v>2</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
@@ -1596,15 +1711,15 @@
         <v>2</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
@@ -1613,23 +1728,23 @@
         <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>2</v>
@@ -1637,10 +1752,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>2</v>
@@ -1648,10 +1763,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>2</v>
@@ -1659,10 +1774,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>2</v>
@@ -1670,10 +1785,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>2</v>
@@ -1681,10 +1796,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>2</v>
@@ -1692,10 +1807,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>2</v>
@@ -1703,24 +1818,24 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>2</v>
@@ -1728,10 +1843,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>2</v>
@@ -1739,10 +1854,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>2</v>
@@ -1750,7 +1865,7 @@
     </row>
     <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1758,7 +1873,7 @@
         <v>22</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -1772,22 +1887,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F64" s="1" t="s">
-        <v>89</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F65" s="1" t="s">
-        <v>84</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F66" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F67" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -1832,10 +1947,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
@@ -1846,15 +1961,15 @@
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
       <c r="H77" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>8</v>
@@ -1865,15 +1980,15 @@
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
       <c r="H78" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
@@ -1886,10 +2001,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
@@ -1898,15 +2013,15 @@
         <v>2</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -1920,10 +2035,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
@@ -1932,17 +2047,17 @@
         <v>2</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F83" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>32</v>
@@ -1954,15 +2069,15 @@
         <v>2</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>32</v>
@@ -1974,15 +2089,15 @@
         <v>2</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>32</v>
@@ -1994,38 +2109,38 @@
         <v>2</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F87" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F88" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F89" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
@@ -2039,15 +2154,15 @@
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>8</v>
@@ -2061,10 +2176,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>8</v>
@@ -2075,10 +2190,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>8</v>
@@ -2090,23 +2205,23 @@
         <v>2</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F97" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>8</v>
@@ -2120,16 +2235,16 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>2</v>
@@ -2137,13 +2252,13 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>2</v>
@@ -2151,18 +2266,18 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>8</v>
@@ -2174,15 +2289,15 @@
         <v>2</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>8</v>
@@ -2194,40 +2309,40 @@
         <v>2</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D104" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F104" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="H104" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>8</v>
@@ -2241,27 +2356,27 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>8</v>
@@ -2270,41 +2385,83 @@
         <v>2</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H112" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>216</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2315,11 +2472,247 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.85546875" customWidth="1"/>
+    <col min="2" max="2" width="94" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" customWidth="1"/>
+    <col min="8" max="8" width="68" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2340,7 +2733,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>224</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -2358,31 +2751,31 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -2391,7 +2784,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2403,7 +2796,7 @@
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -2418,7 +2811,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I4" s="1">
         <v>10</v>
@@ -2433,15 +2826,15 @@
         <v>72</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -2456,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -2471,15 +2864,15 @@
         <v>254</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -2494,7 +2887,7 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -2512,15 +2905,15 @@
         <v>4</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
@@ -2535,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2553,15 +2946,15 @@
         <v>5</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -2576,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>

</xml_diff>

<commit_message>
new semantical tests added; docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="269">
   <si>
     <t>Static Error?</t>
   </si>
@@ -793,10 +793,46 @@
     <t>Integration: P semantics test: one machine, "push", "send" in entry and exit</t>
   </si>
   <si>
-    <t>SEM_OneMachine_11\PushImplicitPop.p</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, "push" with implicit "pop"</t>
+    <t>Integration: P semantics test: one machine, "push" with explicit "pop"</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_13\PushTransInheritance.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "push" transition, action inherited by the pushed state</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_12\PushExplicitPop.2</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "goto" transition, action is not inherited by the destination state</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_14\GotoTransInheritance.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_15\ImplicitPopExit.p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration: P semantics test: one machine, exit actions executed upon implicit "pop" </t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_16\ExplicitPopExit.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_17\PushImplicitPopWithRaise.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_11\PushImplicitPopWithSend.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "push" with implicit "pop" when the unhandled event was sent</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, exit actions executed upon explicit "pop"</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "push" with implicit "pop" when the unhandled event was raised</t>
   </si>
 </sst>
 </file>
@@ -2472,16 +2508,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.85546875" customWidth="1"/>
-    <col min="2" max="2" width="94" customWidth="1"/>
+    <col min="2" max="2" width="97.5703125" customWidth="1"/>
     <col min="6" max="6" width="43.5703125" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" customWidth="1"/>
     <col min="8" max="8" width="68" customWidth="1"/>
@@ -2691,16 +2727,103 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" t="s">
         <v>255</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>256</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
+      <c r="B15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>261</v>
+      </c>
+      <c r="B17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new semantical and liveness tests added; docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
     <sheet name="NewSemTests" sheetId="3" r:id="rId2"/>
-    <sheet name="SamplesProtocols" sheetId="2" r:id="rId3"/>
+    <sheet name="Liveness" sheetId="4" r:id="rId3"/>
+    <sheet name="SamplesProtocols" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="281">
   <si>
     <t>Static Error?</t>
   </si>
@@ -833,6 +834,42 @@
   </si>
   <si>
     <t>Integration: P semantics test: one machine, "push" with implicit "pop" when the unhandled event was raised</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_18\UnhandledEventDeferred.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, deferral of an unhandled event</t>
+  </si>
+  <si>
+    <t>Liveness_1.p</t>
+  </si>
+  <si>
+    <t>Liveness:  simplest sample demonstrating liveness checking</t>
+  </si>
+  <si>
+    <t>Liveness_1_falsePass.p</t>
+  </si>
+  <si>
+    <t>Liveness: sample demonstrating "false" pass in liveness checking</t>
+  </si>
+  <si>
+    <t>TODO: need to issue a warning (or error); compare this test to Liveness_1.p</t>
+  </si>
+  <si>
+    <t>Liveness_2.p</t>
+  </si>
+  <si>
+    <t>Liveness_2_bugFound.p</t>
+  </si>
+  <si>
+    <t>Liveness: sample demonstrating demonstrating liveness error found</t>
+  </si>
+  <si>
+    <t>"check passed", but expected to fail; TODO: bug in liveness checking in Zing</t>
+  </si>
+  <si>
+    <t>No(wrong!)</t>
   </si>
 </sst>
 </file>
@@ -2508,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,7 +2818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>261</v>
       </c>
@@ -2795,7 +2832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>263</v>
       </c>
@@ -2809,7 +2846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>264</v>
       </c>
@@ -2824,6 +2861,26 @@
       </c>
       <c r="F19" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2832,6 +2889,123 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>

</xml_diff>

<commit_message>
testing docs updated, new test added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="286">
   <si>
     <t>Static Error?</t>
   </si>
@@ -876,6 +876,15 @@
   </si>
   <si>
     <t>Liveness: Liveness bug detected with the target thread blocked (no deadlock)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  </t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_19\UnhandledEventIgnored.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "ignore" of an unhandled event</t>
   </si>
 </sst>
 </file>
@@ -2551,10 +2560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,7 +2577,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>224</v>
+        <v>283</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -2887,6 +2896,23 @@
       </c>
       <c r="H20" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>284</v>
+      </c>
+      <c r="B21" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2898,7 +2924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new tests added, docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="293">
   <si>
     <t>Static Error?</t>
   </si>
@@ -885,6 +885,27 @@
   </si>
   <si>
     <t>Integration: P semantics test: one machine, "ignore" of an unhandled event</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_21\BugReproIdenticalTerms_workaround.p</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_20\BugReproIdenticalTerms.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, exit function performed while explicitly popping the state</t>
+  </si>
+  <si>
+    <t>Bug repro: Zinger line number reporting is wrong</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_22\AlonBug_1.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, deadlocked state is not the only state on the stack</t>
+  </si>
+  <si>
+    <t>Compare with AlonBug.p</t>
   </si>
 </sst>
 </file>
@@ -1234,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A94" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,10 +2581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,6 +2936,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>287</v>
+      </c>
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23" t="s">
+        <v>288</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2924,7 +2996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
regression tool fixed for runtime; runtime tests added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="297">
   <si>
     <t>Static Error?</t>
   </si>
@@ -485,9 +485,6 @@
     <t xml:space="preserve">1.6.2. Undefined function for exit </t>
   </si>
   <si>
-    <t>"model functions can be declared only in real machines"; "Nondeterminitistic choice can be used only in model machine and model functions" (both cases tested); ""if (...)" expects a boolean value";</t>
-  </si>
-  <si>
     <t>"argument 1 of "raise" expects an event value"; "argument 2 of "send" expects an event value"</t>
   </si>
   <si>
@@ -500,9 +497,6 @@
     <t xml:space="preserve">"invalid payload type in raise"; "invalid payload type in send"; "invalid assignment. right hand side is not a subtype of left hand side"; </t>
   </si>
   <si>
-    <t>"model functions can be declared only in real machines"; "default transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side";</t>
-  </si>
-  <si>
     <t>"No Main Machine"; "no start state in machine", "function cannot take arguments" (for entry and exit); “Bad field name"; "Operator expected first argument to be an integer value"; "invalid assignment. right hand side is not a subtype of left hand side";</t>
   </si>
   <si>
@@ -866,12 +860,6 @@
     <t>Liveness: sample demonstrating demonstrating liveness error found</t>
   </si>
   <si>
-    <t>"check passed", but expected to fail; TODO: bug in liveness checking in Zing</t>
-  </si>
-  <si>
-    <t>No(wrong!)</t>
-  </si>
-  <si>
     <t>Liveness_3</t>
   </si>
   <si>
@@ -921,6 +909,15 @@
   </si>
   <si>
     <t>to validate test EventSentAfterSentHalt.p</t>
+  </si>
+  <si>
+    <t>"check failed", because there's a deadlock.  TODO: Ask Shaz to confirm that this is a correct result.</t>
+  </si>
+  <si>
+    <t>"default transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side";</t>
+  </si>
+  <si>
+    <t>"Nondeterminitistic choice can be used only in model machine and model functions" (both cases tested); ""if (...)" expects a boolean value";</t>
   </si>
 </sst>
 </file>
@@ -1270,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A94" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1286,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -1420,7 +1417,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>152</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1457,7 +1454,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1474,7 +1471,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1501,7 +1498,7 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1554,7 +1551,7 @@
         <v>81</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>157</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1567,7 +1564,7 @@
         <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -1579,7 +1576,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1624,7 +1621,7 @@
         <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
@@ -1647,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1655,7 +1652,7 @@
         <v>121</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>99</v>
@@ -1664,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1681,7 +1678,7 @@
         <v>124</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,7 +1738,7 @@
         <v>136</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1753,7 +1750,7 @@
         <v>2</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1775,15 +1772,15 @@
     </row>
     <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
@@ -1795,15 +1792,15 @@
         <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
@@ -1815,15 +1812,15 @@
         <v>2</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
@@ -1835,15 +1832,15 @@
         <v>2</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
@@ -1855,20 +1852,20 @@
         <v>79</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>2</v>
@@ -1876,10 +1873,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>2</v>
@@ -1887,10 +1884,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>2</v>
@@ -1898,10 +1895,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>2</v>
@@ -1909,10 +1906,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>2</v>
@@ -1920,10 +1917,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>2</v>
@@ -1931,10 +1928,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>2</v>
@@ -1942,24 +1939,24 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>2</v>
@@ -1967,10 +1964,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>2</v>
@@ -1978,10 +1975,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>2</v>
@@ -2011,12 +2008,12 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F64" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F65" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2142,10 +2139,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -2162,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
@@ -2317,7 +2314,7 @@
         <v>42</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>8</v>
@@ -2390,10 +2387,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -2401,7 +2398,7 @@
         <v>44</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>8</v>
@@ -2421,7 +2418,7 @@
         <v>57</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>8</v>
@@ -2441,7 +2438,7 @@
         <v>58</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>8</v>
@@ -2480,24 +2477,24 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>99</v>
@@ -2509,15 +2506,15 @@
         <v>2</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>99</v>
@@ -2526,15 +2523,15 @@
         <v>2</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>99</v>
@@ -2543,49 +2540,49 @@
         <v>2</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2598,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2613,7 +2610,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -2639,10 +2636,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2651,15 +2648,15 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2671,15 +2668,15 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2688,15 +2685,15 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -2710,10 +2707,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -2722,21 +2719,21 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" t="s">
         <v>230</v>
-      </c>
-      <c r="G7" t="s">
-        <v>233</v>
-      </c>
-      <c r="H7" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -2745,15 +2742,15 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2765,15 +2762,15 @@
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2784,27 +2781,27 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
         <v>250</v>
-      </c>
-      <c r="B11" t="s">
-        <v>251</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2815,10 +2812,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -2829,10 +2826,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -2843,10 +2840,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -2857,10 +2854,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -2871,10 +2868,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -2885,10 +2882,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -2899,10 +2896,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -2911,15 +2908,15 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -2931,15 +2928,15 @@
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -2953,10 +2950,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B22" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -2965,15 +2962,15 @@
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B23" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -2984,10 +2981,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B24" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -2999,15 +2996,15 @@
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B25" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -3021,19 +3018,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B26" t="s">
+        <v>289</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
         <v>293</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" t="s">
-        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3045,14 +3042,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="67.85546875" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="35.7109375" customWidth="1"/>
     <col min="7" max="7" width="47.7109375" customWidth="1"/>
@@ -3061,7 +3058,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -3087,10 +3084,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3104,30 +3101,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
         <v>273</v>
-      </c>
-      <c r="B4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B5" t="s">
         <v>276</v>
-      </c>
-      <c r="B5" t="s">
-        <v>278</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3138,27 +3135,27 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>280</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C7" t="s">
         <v>99</v>
@@ -3197,7 +3194,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -3221,25 +3218,25 @@
         <v>145</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -3248,7 +3245,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3275,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I4" s="1">
         <v>10</v>
@@ -3290,15 +3287,15 @@
         <v>72</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -3313,7 +3310,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -3328,7 +3325,7 @@
         <v>254</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>79</v>
@@ -3336,7 +3333,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -3351,7 +3348,7 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -3372,12 +3369,12 @@
         <v>79</v>
       </c>
       <c r="O6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
@@ -3392,7 +3389,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -3413,12 +3410,12 @@
         <v>79</v>
       </c>
       <c r="O7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -3433,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>

</xml_diff>

<commit_message>
updates in the regression tool (better parsing of input pars)
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
-    <sheet name="NewSemTests" sheetId="3" r:id="rId2"/>
-    <sheet name="Liveness" sheetId="4" r:id="rId3"/>
-    <sheet name="SamplesProtocols" sheetId="2" r:id="rId4"/>
+    <sheet name="Zinger" sheetId="5" r:id="rId2"/>
+    <sheet name="NewSemTests" sheetId="3" r:id="rId3"/>
+    <sheet name="Liveness" sheetId="4" r:id="rId4"/>
+    <sheet name="SamplesProtocols" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="309">
   <si>
     <t>Static Error?</t>
   </si>
@@ -923,10 +924,37 @@
     <t>Actions_6</t>
   </si>
   <si>
-    <t>Feature Integration: payload with push transition</t>
-  </si>
-  <si>
     <t>SEM_TwoMachines_2\EventSentAfterSentHalt_v.p</t>
+  </si>
+  <si>
+    <t>Feature Integration: 1.7.2.3. Payload with push transition</t>
+  </si>
+  <si>
+    <t>BoundedChoice</t>
+  </si>
+  <si>
+    <t>Zinger: testing bounded choice operator in Zing</t>
+  </si>
+  <si>
+    <t>Zinger arg: -bc:2</t>
+  </si>
+  <si>
+    <t>BoundedChoice_1</t>
+  </si>
+  <si>
+    <t>Same as BoundedChoice, but default "-bc" argument for zinger.exe</t>
+  </si>
+  <si>
+    <t>DFSStackBound</t>
+  </si>
+  <si>
+    <t>Zinger: testing DFS stack bound option in Zing</t>
+  </si>
+  <si>
+    <t>"DFS Stack Size Exceeded 10"</t>
+  </si>
+  <si>
+    <t>Zinger args: "-maxdfsstack:10", "-ibound:100"</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2198,7 @@
         <v>297</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -2652,6 +2680,120 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="8" max="8" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>307</v>
+      </c>
+      <c r="I5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
@@ -3130,7 +3272,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B26" t="s">
         <v>288</v>
@@ -3153,7 +3295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -3290,11 +3432,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
regression tests added/modified; test docs updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="315">
   <si>
     <t>Static Error?</t>
   </si>
@@ -955,6 +955,24 @@
   </si>
   <si>
     <t>Zinger args: "-maxdfsstack:10", "-ibound:100"</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>No (non-terminating)</t>
+  </si>
+  <si>
+    <t>Yes? (needs editing)</t>
+  </si>
+  <si>
+    <t>EventDeferredHandledSameState</t>
+  </si>
+  <si>
+    <t>1.6.2.2. Event deferred and handled in the same state</t>
+  </si>
+  <si>
+    <t>"Multiple actions over the same event"</t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,55 +2247,46 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G83" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G84" s="1" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G85" s="1" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>31</v>
@@ -2292,15 +2301,15 @@
         <v>2</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>31</v>
@@ -2311,61 +2320,62 @@
       <c r="D87" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F87" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G87" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I87" s="1" t="s">
+      <c r="I88" s="1" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G88" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G89" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G90" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G91" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>8</v>
@@ -2375,135 +2385,140 @@
       </c>
       <c r="E95" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G97" s="1" t="s">
+      <c r="C98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G98" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I97" s="1" t="s">
+      <c r="I98" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G98" s="1" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G99" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F101" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>200</v>
+        <v>95</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>106</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>167</v>
@@ -2517,13 +2532,16 @@
       <c r="E104" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F104" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G104" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>167</v>
@@ -2532,74 +2550,74 @@
         <v>8</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G105" s="1" t="s">
+      <c r="G106" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I105" s="1" t="s">
+      <c r="I106" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>156</v>
+        <v>8</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>208</v>
+        <v>2</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>167</v>
@@ -2608,15 +2626,18 @@
         <v>98</v>
       </c>
       <c r="D112" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>167</v>
@@ -2628,29 +2649,32 @@
         <v>2</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>215</v>
+        <v>98</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>2</v>
@@ -2661,15 +2685,29 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H116" s="1" t="s">
+      <c r="C117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H117" s="1" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2683,7 +2721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -2798,13 +2836,13 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="2" max="2" width="102.140625" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="43.5703125" customWidth="1"/>
     <col min="8" max="8" width="45.7109375" customWidth="1"/>
@@ -2876,6 +2914,9 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
       <c r="G4" t="s">
         <v>223</v>
       </c>
@@ -2916,6 +2957,9 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2979,6 +3023,9 @@
       <c r="E9" t="s">
         <v>2</v>
       </c>
+      <c r="F9" t="s">
+        <v>311</v>
+      </c>
       <c r="I9" t="s">
         <v>238</v>
       </c>
@@ -3175,6 +3222,9 @@
       <c r="E20" t="s">
         <v>2</v>
       </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
       <c r="I20" t="s">
         <v>229</v>
       </c>
@@ -3195,6 +3245,9 @@
       <c r="E21" t="s">
         <v>2</v>
       </c>
+      <c r="F21" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -3247,6 +3300,9 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
         <v>2</v>
       </c>
       <c r="I24" t="s">

</xml_diff>

<commit_message>
new semantics tests added, dics updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="321">
   <si>
     <t>Static Error?</t>
   </si>
@@ -894,12 +894,6 @@
     <t>Compare with AlonBug.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: event sent after machine is halted: validating test</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: event sent after machine is halted</t>
-  </si>
-  <si>
     <t>SEM_TwoMachines_1\EventSentAfterSentHalt.p</t>
   </si>
   <si>
@@ -973,6 +967,30 @@
   </si>
   <si>
     <t>"Multiple actions over the same event"</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_25\NewInExit.p</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: one machine, "new" in exit function</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_3\EventSentAfterSentHaltHandled</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is handled</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is not handled</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is not handled: validating test</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_4\EventSentAfterSentHaltHandled_v</t>
+  </si>
+  <si>
+    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is handled: validating test</t>
   </si>
 </sst>
 </file>
@@ -1322,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1375,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1476,7 +1494,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1610,7 +1628,7 @@
         <v>80</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2050,7 +2068,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>81</v>
@@ -2213,10 +2231,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -2247,16 +2265,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -2471,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -2533,7 +2551,7 @@
         <v>2</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>106</v>
@@ -2751,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -2765,30 +2783,30 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
         <v>300</v>
-      </c>
-      <c r="B3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2800,30 +2818,30 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
         <v>305</v>
       </c>
-      <c r="B5" t="s">
+      <c r="I5" t="s">
         <v>306</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>307</v>
-      </c>
-      <c r="I5" t="s">
-        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -2833,10 +2851,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,7 +2884,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -3024,7 +3042,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I9" t="s">
         <v>238</v>
@@ -3246,7 +3264,7 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3311,39 +3329,93 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B26" t="s">
-        <v>288</v>
+        <v>317</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>2</v>
-      </c>
-      <c r="I26" t="s">
-        <v>291</v>
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>296</v>
+      </c>
+      <c r="B27" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B28" t="s">
+        <v>316</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>319</v>
+      </c>
+      <c r="B29" t="s">
+        <v>320</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>307</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3386,7 +3458,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -3466,7 +3538,7 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
regression tool fixed for capturing error output; new tests added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
-    <sheet name="Zinger" sheetId="5" r:id="rId2"/>
-    <sheet name="NewSemTests" sheetId="3" r:id="rId3"/>
-    <sheet name="Liveness" sheetId="4" r:id="rId4"/>
-    <sheet name="SamplesProtocols" sheetId="2" r:id="rId5"/>
+    <sheet name="Runtime" sheetId="6" r:id="rId2"/>
+    <sheet name="Zinger" sheetId="5" r:id="rId3"/>
+    <sheet name="NewSemTests" sheetId="3" r:id="rId4"/>
+    <sheet name="Liveness" sheetId="4" r:id="rId5"/>
+    <sheet name="SamplesProtocols" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="348">
   <si>
     <t>Static Error?</t>
   </si>
@@ -747,69 +748,30 @@
     <t>Compare to SEM_OneMachine_5\SendInExitUnhandledEvent.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine,  "send" to itself and "raise" in entry actions</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, 'raise" and "send" to itself in entry actions</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, "send" to itself in entry actions</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine,"send" to itself in exit not executed</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine,  "send" to itself in exit function</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, "send" to itself in exit function</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_8\GotoToItself.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "goto" to the same state; "send" in entry and exit</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_9\PushItself.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "push" and "goto" to the same state; "send" in entry and exit</t>
-  </si>
-  <si>
     <t>1.1.1.2. Assert Max Instances of an event</t>
   </si>
   <si>
     <t>SEM_OneMachine_10\Push.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "push", "send" in entry and exit</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, "push" with explicit "pop"</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_13\PushTransInheritance.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "push" transition, action inherited by the pushed state</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_12\PushExplicitPop.2</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "goto" transition, action is not inherited by the destination state</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_14\GotoTransInheritance.p</t>
   </si>
   <si>
     <t>SEM_OneMachine_15\ImplicitPopExit.p</t>
   </si>
   <si>
-    <t xml:space="preserve">Integration: P semantics test: one machine, exit actions executed upon implicit "pop" </t>
-  </si>
-  <si>
     <t>SEM_OneMachine_16\ExplicitPopExit.p</t>
   </si>
   <si>
@@ -819,21 +781,9 @@
     <t>SEM_OneMachine_11\PushImplicitPopWithSend.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "push" with implicit "pop" when the unhandled event was sent</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, exit actions executed upon explicit "pop"</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: one machine, "push" with implicit "pop" when the unhandled event was raised</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_18\UnhandledEventDeferred.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, deferral of an unhandled event</t>
-  </si>
-  <si>
     <t>Liveness_1.p</t>
   </si>
   <si>
@@ -870,27 +820,18 @@
     <t>SEM_OneMachine_19\UnhandledEventIgnored.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "ignore" of an unhandled event</t>
-  </si>
-  <si>
     <t>SEM_OneMachine_21\BugReproIdenticalTerms_workaround.p</t>
   </si>
   <si>
     <t>SEM_OneMachine_20\BugReproIdenticalTerms.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, exit function performed while explicitly popping the state</t>
-  </si>
-  <si>
     <t>Bug repro: Zinger line number reporting is wrong</t>
   </si>
   <si>
     <t>SEM_OneMachine_22\AlonBug_1.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, deadlocked state is not the only state on the stack</t>
-  </si>
-  <si>
     <t>Compare with AlonBug.p</t>
   </si>
   <si>
@@ -972,25 +913,166 @@
     <t>SEM_OneMachine_25\NewInExit.p</t>
   </si>
   <si>
-    <t>Integration: P semantics test: one machine, "new" in exit function</t>
-  </si>
-  <si>
     <t>SEM_TwoMachines_3\EventSentAfterSentHaltHandled</t>
   </si>
   <si>
-    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is handled</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is not handled</t>
-  </si>
-  <si>
-    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is not handled: validating test</t>
-  </si>
-  <si>
     <t>SEM_TwoMachines_4\EventSentAfterSentHaltHandled_v</t>
   </si>
   <si>
-    <t>Integration: P semantics test: two machines, event sent after "halt", "halt" is handled: validating test</t>
+    <t>Liveness_2_WarmState</t>
+  </si>
+  <si>
+    <t>Liveness: "warm" state instead of "hot"</t>
+  </si>
+  <si>
+    <t>Liveness_1_WarmState</t>
+  </si>
+  <si>
+    <t>Liveness: "warm" state instead of "cold"</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_24\TopHandlerOverridesInherited</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_23\TopHandlerOverridesInherited_v</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_26\TopHandlerOverrides</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_27\TopHandlerOverrides_v</t>
+  </si>
+  <si>
+    <t>1.6.6.1. Multiple handlers for the event: ignore/defer case</t>
+  </si>
+  <si>
+    <t>DeferIgnore1</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine,  "send" to itself and "raise" in entry actions</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, 'raise" and "send" to itself in entry actions</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "send" to itself in entry actions</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine,"send" to itself in exit not executed</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine,  "send" to itself in exit function</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "send" to itself in exit function</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "goto" to the same state; "send" in entry and exit</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "push" and "goto" to the same state; "send" in entry and exit</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "push", "send" in entry and exit</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "push" with implicit "pop" when the unhandled event was sent</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "push" with explicit "pop"</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "push" transition, action inherited by the pushed state</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "goto" transition, action is not inherited by the destination state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P semantics test: one machine, exit actions executed upon implicit "pop" </t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, exit actions executed upon explicit "pop"</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "push" with implicit "pop" when the unhandled event was raised</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, deferral of an unhandled event</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "ignore" of an unhandled event</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, exit function performed while explicitly popping the state</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, deadlocked state is not the only state on the stack</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, inherited handler for event overriden by "defer"</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "new" in exit function</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, inherited handler for event overriden by "ignore"</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, event sent after "halt", "halt" is not handled</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, event sent after "halt", "halt" is not handled: validating test</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, event sent after "halt", "halt" is handled</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, event sent after "halt", "halt" is handled: validating test</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_28\DeferIgnore2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deferred event is never handled, </t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, asgn to uninitialized sequence (runtime error)</t>
+  </si>
+  <si>
+    <t>Yes (error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enabled error messages </t>
+  </si>
+  <si>
+    <t>Enabled error messages</t>
+  </si>
+  <si>
+    <t>Runtime: "ASSERT: Invalid index";    Zinger: "Expression: assert(0 &lt;= index &amp;&amp; index &lt; size)"</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_40\lvalues_runtimeError</t>
+  </si>
+  <si>
+    <t>functionAnyAnon</t>
+  </si>
+  <si>
+    <t>1.5: anonymous function cannot return a value</t>
+  </si>
+  <si>
+    <t>"anonymous function cannot return a value"</t>
+  </si>
+  <si>
+    <t>validating test for OneMachine_24</t>
+  </si>
+  <si>
+    <t>validating test for OneMachine_26</t>
+  </si>
+  <si>
+    <t>P semantics test, one machine: "defer" semantics and the state stack</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_29\DeferIgnore3</t>
   </si>
 </sst>
 </file>
@@ -1338,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="H119" sqref="H119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1457,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1494,7 +1576,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1628,7 +1710,7 @@
         <v>80</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2068,7 +2150,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>81</v>
@@ -2231,10 +2313,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -2265,16 +2347,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -2489,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -2551,7 +2633,7 @@
         <v>2</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>106</v>
@@ -2727,6 +2809,34 @@
       </c>
       <c r="H117" s="1" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2737,10 +2847,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" customWidth="1"/>
+    <col min="9" max="9" width="59.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,13 +2934,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>143</v>
+        <v>338</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>144</v>
@@ -2783,10 +2948,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2798,15 +2963,15 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2818,15 +2983,15 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2838,10 +3003,10 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="I5" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2849,19 +3014,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.85546875" customWidth="1"/>
     <col min="2" max="2" width="102.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="43.5703125" customWidth="1"/>
     <col min="8" max="8" width="45.7109375" customWidth="1"/>
     <col min="9" max="9" width="68" customWidth="1"/>
@@ -2869,7 +3034,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -2884,7 +3049,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -2901,7 +3066,7 @@
         <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>306</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2921,7 +3086,7 @@
         <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>307</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2944,7 +3109,7 @@
         <v>233</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>308</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2964,7 +3129,7 @@
         <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>309</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -2984,7 +3149,7 @@
         <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>310</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -3010,7 +3175,7 @@
         <v>236</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>311</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3030,7 +3195,7 @@
         <v>237</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>311</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3042,7 +3207,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="I9" t="s">
         <v>238</v>
@@ -3050,10 +3215,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>312</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3067,10 +3232,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>313</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3082,15 +3247,15 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>251</v>
+        <v>314</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3104,10 +3269,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>315</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3121,10 +3286,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>252</v>
+        <v>316</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3138,10 +3303,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>317</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3155,10 +3320,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>318</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3172,10 +3337,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>319</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3189,10 +3354,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>320</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3206,10 +3371,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>321</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3221,15 +3386,15 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>322</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -3249,10 +3414,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="B21" t="s">
-        <v>280</v>
+        <v>323</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3264,15 +3429,15 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3284,15 +3449,15 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B23" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3306,10 +3471,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -3324,15 +3489,15 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="B25" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -3342,14 +3507,17 @@
       </c>
       <c r="F25" t="s">
         <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B26" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -3358,15 +3526,18 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B27" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -3376,17 +3547,14 @@
       </c>
       <c r="F27" t="s">
         <v>2</v>
-      </c>
-      <c r="I27" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -3403,18 +3571,152 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>307</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>333</v>
+      </c>
+      <c r="B30" t="s">
+        <v>346</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>347</v>
+      </c>
+      <c r="B31" t="s">
+        <v>346</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B33" t="s">
+        <v>335</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>336</v>
+      </c>
+      <c r="H33" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>268</v>
+      </c>
+      <c r="B36" t="s">
+        <v>329</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>276</v>
+      </c>
+      <c r="B37" t="s">
+        <v>330</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38" t="s">
+        <v>331</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B39" t="s">
+        <v>332</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>287</v>
+      </c>
+      <c r="F39" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3423,12 +3725,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,7 +3760,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -3472,10 +3774,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3489,10 +3791,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3504,15 +3806,15 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3523,10 +3825,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3538,20 +3840,51 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="B7" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="C7" t="s">
         <v>98</v>
       </c>
       <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3560,7 +3893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>

</xml_diff>

<commit_message>
new regression tests added, regression tool updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="361">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1073,6 +1073,45 @@
   </si>
   <si>
     <t>SEM_OneMachine_29\DeferIgnore3</t>
+  </si>
+  <si>
+    <t>this test detected a runtime bug</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_5\RaisedHalt</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, machine is halted with "raise halt" (unhandled)</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_6\RaisedHaltHandled</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, machine is halted with "raise halt" (handled)</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_7\RaisedHalt_bugFound</t>
+  </si>
+  <si>
+    <t>this test found a bug</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_30\DeferIgnore4</t>
+  </si>
+  <si>
+    <t>"unhandled event" exception wrt deferred event</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_31\RaisedHalt</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "halt" is raised and unhandled</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_32\RaisedHaltHandled</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "halt" is raised and handled</t>
   </si>
 </sst>
 </file>
@@ -3016,10 +3055,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,6 +3142,9 @@
       <c r="G4" t="s">
         <v>223</v>
       </c>
+      <c r="I4" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -3626,98 +3668,218 @@
         <v>2</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>355</v>
+      </c>
+      <c r="B32" t="s">
+        <v>346</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="B33" t="s">
-        <v>335</v>
+        <v>358</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>336</v>
-      </c>
-      <c r="H33" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>268</v>
-      </c>
-      <c r="B36" t="s">
-        <v>329</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>276</v>
-      </c>
-      <c r="B37" t="s">
-        <v>330</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>2</v>
-      </c>
-      <c r="I37" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>294</v>
-      </c>
-      <c r="B38" t="s">
-        <v>331</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>359</v>
+      </c>
+      <c r="B34" t="s">
+        <v>360</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>340</v>
+      </c>
+      <c r="B39" t="s">
+        <v>335</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>336</v>
+      </c>
+      <c r="H39" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>268</v>
+      </c>
+      <c r="B42" t="s">
+        <v>329</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>276</v>
+      </c>
+      <c r="B43" t="s">
+        <v>330</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>294</v>
+      </c>
+      <c r="B44" t="s">
+        <v>331</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>295</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
         <v>332</v>
       </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>287</v>
-      </c>
-      <c r="F39" t="s">
-        <v>2</v>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>349</v>
+      </c>
+      <c r="B46" t="s">
+        <v>350</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>351</v>
+      </c>
+      <c r="B47" t="s">
+        <v>352</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>353</v>
+      </c>
+      <c r="B48" t="s">
+        <v>350</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regression updated; new tests added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="433">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1285,13 +1285,49 @@
     <t xml:space="preserve">tuple with map: accessing element by non-existing key </t>
   </si>
   <si>
-    <t>failed: Zinger: "P Assertion failed: Expression: assert(false)"; runtime: "ERROR: ASSERT: Invalid map get; key not found"</t>
-  </si>
-  <si>
-    <t>??failed (Zinger and runtime): assert(0 &lt;= index &amp;&amp; index &lt; size)</t>
-  </si>
-  <si>
-    <t>??Runtime: "ERROR: ASSERT: Invalid map get; key not found"; zinger: "Error: P Assertion failed: Expression: assert(false)"</t>
+    <t>Runtime: "ASSERT: Invalid index"; Zinger: "Expression: assert(0 &lt;= index &amp;&amp; index &lt; size); Comment: index out of bound"</t>
+  </si>
+  <si>
+    <t>Runtime: "ERROR: ASSERT: Invalid map get; key not found"; zinger: "Error: P Assertion failed: Expression: assert(false); Comment: key not found"</t>
+  </si>
+  <si>
+    <t>??Runtime(crashing after recent changes): "ERROR: ASSERT: Invalid map get; key not found"; zinger: "Error: P Assertion failed: Expression: assert(false); Comment: key not found"</t>
+  </si>
+  <si>
+    <t>failed: Zinger: "P Assertion failed: Expression: assert(false); Comment: key not found"; runtime (crashing after recent changes): "ERROR: ASSERT: Invalid map get; key not found"</t>
+  </si>
+  <si>
+    <t>DynamicError\nonAtomicDataTypes12</t>
+  </si>
+  <si>
+    <t>this test caused StackOverflowException in pc.exe (fixed)</t>
+  </si>
+  <si>
+    <t>runtime crashes</t>
+  </si>
+  <si>
+    <t>runtime crashes; Zinger: "P Assertion failed: Expression: assert(0 &lt;= index &amp;&amp; index &lt; size); Comment: index out of bound"</t>
+  </si>
+  <si>
+    <t>DynamicError\nonAtomicDataTypes13</t>
+  </si>
+  <si>
+    <t>this test caused pc.exe error on line 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the most comprehensive "Correct" test </t>
+  </si>
+  <si>
+    <t>the most comprehensive "StaticError" test</t>
+  </si>
+  <si>
+    <t>"invalid assignment. right hand side is not a subtype of left hand side", "insert must be applied to a sequence or a map", "remove must be applied to a sequence or map", "Bad field name", "index must be an integer", "invalid LHS; must have the form LHS ::= var | LHS[expr] | LHS.name", ""in" expects a map", "Value can never be in the map"</t>
+  </si>
+  <si>
+    <t>DynamicError\nonAtomicDataTypes14</t>
+  </si>
+  <si>
+    <t>maps: "in" returns "false"</t>
   </si>
 </sst>
 </file>
@@ -1639,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I145"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="H140" sqref="H140"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,6 +3211,12 @@
       <c r="C128" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G128" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
@@ -3310,8 +3352,8 @@
       <c r="G135" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="H135" s="8" t="s">
-        <v>419</v>
+      <c r="H135" s="1" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -3333,8 +3375,8 @@
       <c r="G136" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="H136" s="8" t="s">
-        <v>420</v>
+      <c r="H136" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -3426,27 +3468,108 @@
         <v>417</v>
       </c>
       <c r="H140" s="8" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="H141" s="8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H143" s="8"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H144" s="8"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>2</v>
+      <c r="C146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new tests added, acceptors updated
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="457">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1240,9 +1240,6 @@
     <t>Insertion of element [2] into sequence of size 1</t>
   </si>
   <si>
-    <t>maps: "keys" applied with index 1 for map of with no element with index 1</t>
-  </si>
-  <si>
     <t>DynamicError\nonAtomicDataTypes7</t>
   </si>
   <si>
@@ -1279,24 +1276,12 @@
     <t>Runtime: "ERROR: ASSERT: Invalid map get; key not found"; zinger: "Error: P Assertion failed: Expression: assert(false); Comment: key not found"</t>
   </si>
   <si>
-    <t>??Runtime(crashing after recent changes): "ERROR: ASSERT: Invalid map get; key not found"; zinger: "Error: P Assertion failed: Expression: assert(false); Comment: key not found"</t>
-  </si>
-  <si>
-    <t>failed: Zinger: "P Assertion failed: Expression: assert(false); Comment: key not found"; runtime (crashing after recent changes): "ERROR: ASSERT: Invalid map get; key not found"</t>
-  </si>
-  <si>
     <t>DynamicError\nonAtomicDataTypes12</t>
   </si>
   <si>
     <t>this test caused StackOverflowException in pc.exe (fixed)</t>
   </si>
   <si>
-    <t>runtime crashes</t>
-  </si>
-  <si>
-    <t>runtime crashes; Zinger: "P Assertion failed: Expression: assert(0 &lt;= index &amp;&amp; index &lt; size); Comment: index out of bound"</t>
-  </si>
-  <si>
     <t>DynamicError\nonAtomicDataTypes13</t>
   </si>
   <si>
@@ -1331,6 +1316,90 @@
   </si>
   <si>
     <t>"default transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side"; "Monitors cannot refer to "this"; "invalid payload type in raise"; "invalid payload type in raise (cannot send null value)"; "Monitors cannot be created with "new""; "Undefined machine type"</t>
+  </si>
+  <si>
+    <t>maps: "keys" applied with index 1 for map with no element with index 1</t>
+  </si>
+  <si>
+    <t>Runtime(crashing after recent changes): "ERROR: ASSERT: Invalid map get; key not found"; zinger: "Error: P Assertion failed: Expression: assert(false); Comment: key not found"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zinger: "P Assertion failed: Expression: assert(0 &lt;= index &amp;&amp; index &lt; size); Comment: index out of bound"</t>
+  </si>
+  <si>
+    <t>failed: Zinger: "P Assertion failed: Expression: assert(false); Comment: key not found"; runtime: "ERROR: ASSERT: Invalid map get; key not found"</t>
+  </si>
+  <si>
+    <t>RaisedDefault</t>
+  </si>
+  <si>
+    <t>1.7.7.  "default" event cannot be sent (parse error)</t>
+  </si>
+  <si>
+    <t>SentDefault</t>
+  </si>
+  <si>
+    <t>1.7.7.  "default" event cannot be declared (parse error)</t>
+  </si>
+  <si>
+    <t>DefaultEventDecl</t>
+  </si>
+  <si>
+    <t>NullEventDecl</t>
+  </si>
+  <si>
+    <t>1.7.7.  "null" event cannot be declared (parse error)</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_36\DefaultHandler1</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "default" handler semantics</t>
+  </si>
+  <si>
+    <t>Testing that default handler is enabled in the simplest case</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_37\DefaultHandler2</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_38\DefaultHandlerInheritedByPushTr</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_39\TopDefaultHandlerOverridesInherited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug in Zing; testing top  "default" event handler overriding inherited (by push transition)  handler </t>
+  </si>
+  <si>
+    <t>PtoZingBugFound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug in Zing; the test demonstrates that "default" event handler is executed in a loop </t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_41\DefaultHandlerInLoop</t>
+  </si>
+  <si>
+    <t>1.7.2.2. "goto" transition</t>
+  </si>
+  <si>
+    <t>This test found a bug in P-to-Zing compiler (fixed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug in Zing; testing inherited (by push transition)  "do" on default </t>
+  </si>
+  <si>
+    <t>DeferredDefault</t>
+  </si>
+  <si>
+    <t>1.7.7.  "default" event cannot be deferred (parse error)</t>
+  </si>
+  <si>
+    <t>IgnoredDefault</t>
+  </si>
+  <si>
+    <t>1.7.7.  "default" event cannot be "ignored" (parse error)</t>
   </si>
 </sst>
 </file>
@@ -1678,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,7 +1968,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1962,7 +2031,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1979,7 +2048,7 @@
         <v>78</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2072,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2138,7 +2207,7 @@
         <v>128</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3215,10 +3284,10 @@
         <v>2</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3353,15 +3422,15 @@
         <v>2</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>403</v>
+        <v>429</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>395</v>
@@ -3376,15 +3445,15 @@
         <v>2</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>395</v>
@@ -3399,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>397</v>
@@ -3407,7 +3476,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>395</v>
@@ -3422,15 +3491,15 @@
         <v>2</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="H138" s="8" t="s">
-        <v>416</v>
+        <v>408</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>395</v>
@@ -3445,7 +3514,7 @@
         <v>2</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>397</v>
@@ -3453,7 +3522,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>395</v>
@@ -3468,15 +3537,15 @@
         <v>2</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="H140" s="8" t="s">
-        <v>417</v>
+        <v>412</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>395</v>
@@ -3491,15 +3560,15 @@
         <v>2</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="H141" s="8" t="s">
-        <v>421</v>
+        <v>416</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>395</v>
@@ -3514,21 +3583,15 @@
         <v>2</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H143" s="8"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H144" s="8"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>395</v>
@@ -3546,10 +3609,10 @@
         <v>2</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>393</v>
       </c>
@@ -3569,10 +3632,96 @@
         <v>2</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I157" s="1" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3766,10 +3915,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4496,12 +4645,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>440</v>
+      </c>
+      <c r="B38" t="s">
+        <v>441</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>442</v>
+      </c>
+    </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>333</v>
+        <v>443</v>
       </c>
       <c r="B39" t="s">
-        <v>328</v>
+        <v>441</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -4510,95 +4679,98 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>329</v>
-      </c>
-      <c r="H39" t="s">
-        <v>332</v>
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>262</v>
+        <v>333</v>
       </c>
       <c r="B42" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="s">
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>269</v>
-      </c>
-      <c r="B43" t="s">
-        <v>323</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" t="s">
-        <v>2</v>
-      </c>
-      <c r="I43" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>287</v>
-      </c>
-      <c r="B44" t="s">
-        <v>324</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>288</v>
-      </c>
-      <c r="B45" t="s">
-        <v>325</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" t="s">
-        <v>2</v>
+        <v>329</v>
+      </c>
+      <c r="H42" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>342</v>
+        <v>262</v>
       </c>
       <c r="B46" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -4615,10 +4787,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>344</v>
+        <v>269</v>
       </c>
       <c r="B47" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -4628,48 +4800,125 @@
       </c>
       <c r="F47" t="s">
         <v>2</v>
+      </c>
+      <c r="I47" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" t="s">
+        <v>324</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>288</v>
+      </c>
+      <c r="B49" t="s">
+        <v>325</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>342</v>
+      </c>
+      <c r="B50" t="s">
+        <v>343</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>344</v>
+      </c>
+      <c r="B51" t="s">
+        <v>345</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>346</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" t="s">
         <v>343</v>
       </c>
-      <c r="C48" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" t="s">
-        <v>2</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2</v>
+      </c>
+      <c r="I52" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>373</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>374</v>
       </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"default" -> "null" (for events); new tests added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="458">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1330,45 +1330,18 @@
     <t>failed: Zinger: "P Assertion failed: Expression: assert(false); Comment: key not found"; runtime: "ERROR: ASSERT: Invalid map get; key not found"</t>
   </si>
   <si>
-    <t>RaisedDefault</t>
-  </si>
-  <si>
-    <t>1.7.7.  "default" event cannot be sent (parse error)</t>
-  </si>
-  <si>
-    <t>SentDefault</t>
-  </si>
-  <si>
-    <t>1.7.7.  "default" event cannot be declared (parse error)</t>
-  </si>
-  <si>
-    <t>DefaultEventDecl</t>
-  </si>
-  <si>
     <t>NullEventDecl</t>
   </si>
   <si>
     <t>1.7.7.  "null" event cannot be declared (parse error)</t>
   </si>
   <si>
-    <t>SEM_OneMachine_36\DefaultHandler1</t>
-  </si>
-  <si>
     <t>P semantics test: one machine, "default" handler semantics</t>
   </si>
   <si>
     <t>Testing that default handler is enabled in the simplest case</t>
   </si>
   <si>
-    <t>SEM_OneMachine_37\DefaultHandler2</t>
-  </si>
-  <si>
-    <t>SEM_OneMachine_38\DefaultHandlerInheritedByPushTr</t>
-  </si>
-  <si>
-    <t>SEM_OneMachine_39\TopDefaultHandlerOverridesInherited</t>
-  </si>
-  <si>
     <t xml:space="preserve">bug in Zing; testing top  "default" event handler overriding inherited (by push transition)  handler </t>
   </si>
   <si>
@@ -1378,9 +1351,6 @@
     <t xml:space="preserve">bug in Zing; the test demonstrates that "default" event handler is executed in a loop </t>
   </si>
   <si>
-    <t>SEM_OneMachine_41\DefaultHandlerInLoop</t>
-  </si>
-  <si>
     <t>1.7.2.2. "goto" transition</t>
   </si>
   <si>
@@ -1390,16 +1360,49 @@
     <t xml:space="preserve">bug in Zing; testing inherited (by push transition)  "do" on default </t>
   </si>
   <si>
-    <t>DeferredDefault</t>
-  </si>
-  <si>
-    <t>1.7.7.  "default" event cannot be deferred (parse error)</t>
-  </si>
-  <si>
-    <t>IgnoredDefault</t>
-  </si>
-  <si>
-    <t>1.7.7.  "default" event cannot be "ignored" (parse error)</t>
+    <t>bug in Zing; the test demonstrates that for the "default" event, both payload and trigger are "null"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P semantics test: one machine, payload and trigger for "default" event </t>
+  </si>
+  <si>
+    <t>DeferredNullEvent</t>
+  </si>
+  <si>
+    <t>1.7.7.  "null" event cannot be deferred (parse error)</t>
+  </si>
+  <si>
+    <t>RaisedNullEvent</t>
+  </si>
+  <si>
+    <t>SentNullEvent</t>
+  </si>
+  <si>
+    <t>IgnoredNullEvent</t>
+  </si>
+  <si>
+    <t>1.7.7.  "null" event cannot be sent (parse error)</t>
+  </si>
+  <si>
+    <t>1.7.7.  "null" event cannot be "ignored" (parse error)</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_38\NullHandlerInheritedByPushTr</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_39\TopNullHandlerOverridesInherited</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_41\NullHandlerInLoop</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_42\NullTriggerPayload</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_36\NullEventHandler1</t>
+  </si>
+  <si>
+    <t>SEM_OneMachine_37\NullEventHandler2</t>
   </si>
 </sst>
 </file>
@@ -1747,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,10 +3640,10 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>2</v>
@@ -3648,10 +3651,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>2</v>
@@ -3659,10 +3662,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>2</v>
@@ -3670,10 +3673,10 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>2</v>
@@ -3681,47 +3684,36 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I157" s="1" t="s">
-        <v>451</v>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -3915,10 +3907,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4647,10 +4639,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>440</v>
+        <v>456</v>
       </c>
       <c r="B38" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -4662,180 +4654,183 @@
         <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>457</v>
+      </c>
+      <c r="B39" t="s">
+        <v>435</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="8" t="s">
         <v>443</v>
-      </c>
-      <c r="B39" t="s">
-        <v>441</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>2</v>
-      </c>
-      <c r="F39" t="s">
-        <v>2</v>
-      </c>
-      <c r="I39" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>333</v>
-      </c>
-      <c r="B42" t="s">
-        <v>328</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" t="s">
-        <v>329</v>
-      </c>
-      <c r="H42" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>449</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>262</v>
-      </c>
-      <c r="B46" t="s">
-        <v>322</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
         <v>2</v>
       </c>
       <c r="F47" t="s">
         <v>2</v>
-      </c>
-      <c r="I47" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="B48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" t="s">
         <v>2</v>
       </c>
       <c r="F48" t="s">
         <v>2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B49" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
         <v>2</v>
       </c>
       <c r="F49" t="s">
@@ -4844,18 +4839,15 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>342</v>
+        <v>288</v>
       </c>
       <c r="B50" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
         <v>2</v>
       </c>
       <c r="F50" t="s">
@@ -4864,15 +4856,18 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B51" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
         <v>2</v>
       </c>
       <c r="F51" t="s">
@@ -4881,44 +4876,61 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B52" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" t="s">
         <v>2</v>
       </c>
       <c r="F52" t="s">
         <v>2</v>
-      </c>
-      <c r="I52" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>346</v>
+      </c>
+      <c r="B53" t="s">
+        <v>343</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
+      <c r="I53" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>373</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>374</v>
       </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new tests for non-constant event expressions added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="500">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1306,9 +1306,6 @@
     <t>"transition to an undefined state"; "transition function not defined"; "function cannot take arguments" (for goto transition and do declaration); "action on an undefined event" (for "do" decl); "function not defined" (for "do" decl); "function cannot take arguments" (for "do" decl); "Undeclared state name"; "transition on an undefined event"</t>
   </si>
   <si>
-    <t>"invalid payload type in raise"; "invalid payload type in send"; "invalid assignment. right hand side is not a subtype of left hand side"; "argument 1 of "send" expects a machine value"</t>
-  </si>
-  <si>
     <t>"No Main Machine"; "no start state in machine"; "function requires arguments"; "invalid LHS; must have the form LHS ::= var | LHS[expr] | LHS.name"; "this function must be pure. Data impure functions can only be called like "foo(...);" or "x = foo(...);"; "invalid assignment. right hand side is not a subtype of left hand side"; "function arguments have incorrect types"</t>
   </si>
   <si>
@@ -1403,6 +1400,135 @@
   </si>
   <si>
     <t>SEM_OneMachine_37\NullEventHandler2</t>
+  </si>
+  <si>
+    <t>Liveness_FAIRNONDET\Liveness_FAIRNONDET.p</t>
+  </si>
+  <si>
+    <t>Liveness: NONDET in liveness</t>
+  </si>
+  <si>
+    <t>Liveness_FAIRNONDET\Liveness_FAIRNONDET2.p</t>
+  </si>
+  <si>
+    <t>Liveness: FAIRNONDET in liveness</t>
+  </si>
+  <si>
+    <t>Liveness:FAIR NONDET in liveness</t>
+  </si>
+  <si>
+    <t>Liveness_NONDET\Liveness_NONDET.p</t>
+  </si>
+  <si>
+    <t>Liveness_NONDET\Liveness_NONDET2.p</t>
+  </si>
+  <si>
+    <t>"invalid payload type in raise"; "invalid payload type in send"; "invalid assignment. right hand side is not a subtype of left hand side"; "argument 1 of "send" expects a machine value"; “Undeclared monitor”; "argument 2 of "monitor" expects an event value"</t>
+  </si>
+  <si>
+    <t>eventExprSendRaise</t>
+  </si>
+  <si>
+    <t>2.3.2. "raise" and "send" with non-constant event expression</t>
+  </si>
+  <si>
+    <t>"action on an undefined event"; "argument 2 of "monitor" expects an event value"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no payload </t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, "send", "raise", monitor invocation for non-constant event expressions</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_9\NonConstantEventExpr</t>
+  </si>
+  <si>
+    <t>Zinger: "raised null event" exception</t>
+  </si>
+  <si>
+    <t>runtime: "ASSERT: Raised event must not be null"; Zing: "P Assertion failed: Expression: assert(ev1.ev != null) Comment: (17, 4): Raised null"</t>
+  </si>
+  <si>
+    <t>RaisedNull</t>
+  </si>
+  <si>
+    <t>SentNull</t>
+  </si>
+  <si>
+    <t>Zinger: "sent null event" exception</t>
+  </si>
+  <si>
+    <t>runtime: "ASSERT: Enqueued event must not be null"; Zing: "P Assertion failed: Expression: assert(e != null)  Comment: Comment: Enqueued event must be non-null"</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_10\NonConstantEventExpr1</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines,"send", "raise" with payload for non-constant event expressions</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_11\NonConstantEventExprMonitor</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, monitor invocation with non-constant event expressions</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_12\NonConstantEventExprMonitor1</t>
+  </si>
+  <si>
+    <t>MonitorNull</t>
+  </si>
+  <si>
+    <t>Zinger: monitor invocation with null event expr</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, monitor invocation with non-constant event expression</t>
+  </si>
+  <si>
+    <t>runtime ignores monitor, hence, no error from runtime</t>
+  </si>
+  <si>
+    <t>this test found a bug in Zing (null prt deref, fixed); diff results in Zing and runtime (b/c monitors are ignored in runtime)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">found null ptr deref in Zing (fixed); runtime ignores monitors, hence, no error; Zinger: </t>
+  </si>
+  <si>
+    <t>validating test for Monitor Invocation</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_15\MonitorInvocationEventExprPayload</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, monitor invocation with non-constant event expression with payload</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, monitor instantiation parameter</t>
+  </si>
+  <si>
+    <t>runtime: "ASSERT: id out of bounds"; Zing reports assertion failure in monitor</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_16\NonConstantEventExpr2</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, "send", "raise" with non-constant event expressions</t>
+  </si>
+  <si>
+    <t>diff outputs for runtime and Zing (due to monitors)</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_17\</t>
+  </si>
+  <si>
+    <t>"raise" with non-constant event expression has non-null payload</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_13\NewMonitor</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_14\NewMonitor_v</t>
   </si>
 </sst>
 </file>
@@ -1750,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I156"/>
+  <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2051,7 +2177,7 @@
         <v>78</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2144,7 +2270,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>425</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3290,7 +3416,7 @@
         <v>420</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3425,7 +3551,7 @@
         <v>2</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>413</v>
@@ -3497,7 +3623,7 @@
         <v>408</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -3543,7 +3669,7 @@
         <v>412</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -3566,7 +3692,7 @@
         <v>416</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -3640,10 +3766,10 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>2</v>
@@ -3651,10 +3777,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>2</v>
@@ -3662,10 +3788,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>2</v>
@@ -3673,10 +3799,10 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>2</v>
@@ -3684,36 +3810,53 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B156" s="1" t="s">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I157" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -3779,10 +3922,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3792,6 +3935,7 @@
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="43.140625" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
+    <col min="9" max="9" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -3898,6 +4042,66 @@
       </c>
       <c r="D6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -3907,10 +4111,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4639,50 +4843,50 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B38" t="s">
+        <v>434</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" t="s">
         <v>435</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
-        <v>2</v>
-      </c>
-      <c r="I38" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B39" t="s">
+        <v>434</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
         <v>435</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>2</v>
-      </c>
-      <c r="F39" t="s">
-        <v>2</v>
-      </c>
-      <c r="I39" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
@@ -4694,15 +4898,15 @@
         <v>2</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>7</v>
@@ -4714,7 +4918,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4739,10 +4943,10 @@
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>7</v>
@@ -4754,15 +4958,15 @@
         <v>2</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>7</v>
@@ -4774,7 +4978,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4932,6 +5136,174 @@
       </c>
       <c r="F54" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I62" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I63" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -4941,10 +5313,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5099,6 +5471,68 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B10" t="s">
+        <v>460</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B11" t="s">
+        <v>461</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>462</v>
+      </c>
+      <c r="B12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>463</v>
+      </c>
+      <c r="B13" t="s">
+        <v>458</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed regression (caused by "outputDir" change in pc.exe); new tests added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="517">
   <si>
     <t>Static Error?</t>
   </si>
@@ -64,9 +64,6 @@
     <t>TODO: "function cannot take arguments" -&gt; "function used as entry (exit) action cannot take arguments"</t>
   </si>
   <si>
-    <t>1.8.1.Action on default (no error)</t>
-  </si>
-  <si>
     <t>3.3.4.2. Bad field name</t>
   </si>
   <si>
@@ -1288,9 +1285,6 @@
     <t>this test caused pc.exe error on line 80</t>
   </si>
   <si>
-    <t xml:space="preserve">the most comprehensive "Correct" test </t>
-  </si>
-  <si>
     <t>the most comprehensive "StaticError" test</t>
   </si>
   <si>
@@ -1312,9 +1306,6 @@
     <t>"invalid assignment. right hand side is not a subtype of left hand side", "insert must be applied to a sequence or a map", "remove must be applied to a sequence or map", "Bad field name", "index must be an integer", "invalid LHS; must have the form LHS ::= var | LHS[expr] | LHS.name", ""in" expects a map", "Value can never be in the map"; "Indexer must be applied to a sequence or map"; ""while (...)" expects a boolean value"; "for insert right syntax is seq += (index value) or map += (key value)"</t>
   </si>
   <si>
-    <t>"default transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side"; "Monitors cannot refer to "this"; "invalid payload type in raise"; "invalid payload type in raise (cannot send null value)"; "Monitors cannot be created with "new""; "Undefined machine type"</t>
-  </si>
-  <si>
     <t>maps: "keys" applied with index 1 for map with no element with index 1</t>
   </si>
   <si>
@@ -1333,9 +1324,6 @@
     <t>1.7.7.  "null" event cannot be declared (parse error)</t>
   </si>
   <si>
-    <t>P semantics test: one machine, "default" handler semantics</t>
-  </si>
-  <si>
     <t>Testing that default handler is enabled in the simplest case</t>
   </si>
   <si>
@@ -1357,12 +1345,6 @@
     <t xml:space="preserve">bug in Zing; testing inherited (by push transition)  "do" on default </t>
   </si>
   <si>
-    <t>bug in Zing; the test demonstrates that for the "default" event, both payload and trigger are "null"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P semantics test: one machine, payload and trigger for "default" event </t>
-  </si>
-  <si>
     <t>DeferredNullEvent</t>
   </si>
   <si>
@@ -1519,9 +1501,6 @@
     <t>diff outputs for runtime and Zing (due to monitors)</t>
   </si>
   <si>
-    <t>SEM_TwoMachines_17\</t>
-  </si>
-  <si>
     <t>"raise" with non-constant event expression has non-null payload</t>
   </si>
   <si>
@@ -1529,6 +1508,78 @@
   </si>
   <si>
     <t>SEM_TwoMachines_14\NewMonitor_v</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_17\EventExprSemantics</t>
+  </si>
+  <si>
+    <t>P semantics test: two machines, non-constant event expressions</t>
+  </si>
+  <si>
+    <t>runtime does not detect assert violation (but Zinger does, correctly)</t>
+  </si>
+  <si>
+    <t>Events are sent as payloads of event expressions from Real1 to Real2, and then retrieved in Real2 (into event expression) and sent back to Real1</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_18\EventExprSemantics1</t>
+  </si>
+  <si>
+    <t>runtime does not detect "unhandled event" exception (but Zinger does, correctly)</t>
+  </si>
+  <si>
+    <t>SEM_TwoMachines_19\EventExprSemantics2</t>
+  </si>
+  <si>
+    <t>This test checks using "trigger" as event expression</t>
+  </si>
+  <si>
+    <t>This test enables "Unhandled event" exception</t>
+  </si>
+  <si>
+    <t>ExprOperators</t>
+  </si>
+  <si>
+    <t>3.4. P expressions and operators</t>
+  </si>
+  <si>
+    <t>CastInExprs</t>
+  </si>
+  <si>
+    <t>3.4. Cast operator in expressions</t>
+  </si>
+  <si>
+    <t>DynamicError\nonAtomicDataTypes15\Insert4Map.p</t>
+  </si>
+  <si>
+    <t>maps: INSERT into map with existing index</t>
+  </si>
+  <si>
+    <t>Correct\nonAtomicDataTypesAllAsserts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comprehensive "Correct" test </t>
+  </si>
+  <si>
+    <t>comprehensive "Correct" test with more asserts</t>
+  </si>
+  <si>
+    <t>Runtime: "ERROR: ASSERT: key must not be in map"; zinger: "key must not exist in map"</t>
+  </si>
+  <si>
+    <t>the test demonstrates that for the "default" event, both payload and trigger are "null"</t>
+  </si>
+  <si>
+    <t>P semantics test: one machine, "null" handler semantics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P semantics test: one machine, payload and trigger for "null" event </t>
+  </si>
+  <si>
+    <t>1.8.1.Action on null (no error)</t>
+  </si>
+  <si>
+    <t>"null transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side"; "Monitors cannot refer to "this"; "invalid payload type in raise"; "invalid payload type in raise (cannot send null value)"; "Monitors cannot be created with "new""; "Undefined machine type"</t>
   </si>
 </sst>
 </file>
@@ -1876,15 +1927,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="G155" sqref="G155"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="72.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" style="1" customWidth="1"/>
@@ -1898,10 +1949,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1913,26 +1964,26 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1940,19 +1991,19 @@
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>515</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>5</v>
@@ -1960,41 +2011,41 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -2006,35 +2057,35 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
@@ -2043,12 +2094,12 @@
         <v>8</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -2057,10 +2108,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>10</v>
@@ -2068,76 +2119,76 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
@@ -2151,46 +2202,46 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>427</v>
+        <v>516</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>
@@ -2202,15 +2253,15 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>7</v>
@@ -2222,149 +2273,149 @@
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="H31" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G32" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G33" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G36" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G37" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G38" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G39" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
@@ -2376,15 +2427,15 @@
         <v>2</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>7</v>
@@ -2398,15 +2449,15 @@
     </row>
     <row r="43" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>7</v>
@@ -2418,15 +2469,15 @@
         <v>2</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>7</v>
@@ -2438,15 +2489,15 @@
         <v>2</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>7</v>
@@ -2458,15 +2509,15 @@
         <v>2</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>7</v>
@@ -2475,23 +2526,23 @@
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>2</v>
@@ -2499,10 +2550,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>2</v>
@@ -2510,10 +2561,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>2</v>
@@ -2521,10 +2572,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>2</v>
@@ -2532,10 +2583,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>2</v>
@@ -2543,10 +2594,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>2</v>
@@ -2554,10 +2605,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>2</v>
@@ -2565,24 +2616,24 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>2</v>
@@ -2590,10 +2641,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>2</v>
@@ -2601,10 +2652,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>2</v>
@@ -2612,15 +2663,15 @@
     </row>
     <row r="62" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>7</v>
@@ -2632,75 +2683,75 @@
         <v>2</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G65" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G66" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G67" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G68" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G70" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G71" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G72" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G73" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G74" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G75" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G76" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>7</v>
@@ -2714,15 +2765,15 @@
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>7</v>
@@ -2736,15 +2787,15 @@
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
@@ -2760,30 +2811,30 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>7</v>
@@ -2797,10 +2848,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
@@ -2814,24 +2865,24 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
@@ -2843,20 +2894,20 @@
         <v>2</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G86" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
@@ -2868,18 +2919,18 @@
         <v>2</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>7</v>
@@ -2891,18 +2942,18 @@
         <v>2</v>
       </c>
       <c r="G88" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I88" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>7</v>
@@ -2911,38 +2962,38 @@
         <v>2</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G90" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G91" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G92" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>7</v>
@@ -2956,15 +3007,15 @@
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>7</v>
@@ -2978,10 +3029,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>7</v>
@@ -2995,10 +3046,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>7</v>
@@ -3010,23 +3061,23 @@
         <v>2</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G100" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>7</v>
@@ -3038,21 +3089,21 @@
         <v>2</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>2</v>
@@ -3060,13 +3111,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>2</v>
@@ -3077,18 +3128,18 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>7</v>
@@ -3100,18 +3151,18 @@
         <v>2</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>7</v>
@@ -3123,40 +3174,40 @@
         <v>2</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>7</v>
@@ -3170,27 +3221,27 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="C112" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>7</v>
@@ -3199,232 +3250,232 @@
         <v>2</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="C116" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H116" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="C120" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H120" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H120" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="C121" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H121" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H121" s="1" t="s">
-        <v>356</v>
-      </c>
       <c r="I121" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="C122" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>365</v>
-      </c>
       <c r="C124" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="126" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="C126" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="I126" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="C126" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="I126" s="8" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>7</v>
@@ -3436,18 +3487,18 @@
         <v>2</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>7</v>
@@ -3459,18 +3510,18 @@
         <v>2</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>7</v>
@@ -3482,18 +3533,18 @@
         <v>2</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>7</v>
@@ -3505,18 +3556,18 @@
         <v>2</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>7</v>
@@ -3528,18 +3579,18 @@
         <v>2</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>7</v>
@@ -3551,156 +3602,156 @@
         <v>2</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="H136" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G137" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>406</v>
-      </c>
       <c r="H137" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>408</v>
-      </c>
       <c r="H138" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>410</v>
-      </c>
       <c r="H139" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G140" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>412</v>
-      </c>
       <c r="H140" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>416</v>
-      </c>
       <c r="H141" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>7</v>
@@ -3712,41 +3763,64 @@
         <v>2</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>7</v>
@@ -3761,15 +3835,38 @@
         <v>2</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>419</v>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>2</v>
@@ -3777,10 +3874,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>2</v>
@@ -3788,10 +3885,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>2</v>
@@ -3799,10 +3896,10 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>2</v>
@@ -3810,10 +3907,10 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>2</v>
@@ -3821,27 +3918,27 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>2</v>
@@ -3856,7 +3953,29 @@
         <v>2</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3888,10 +4007,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -3903,16 +4022,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3925,7 +4044,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3940,10 +4059,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -3955,87 +4074,87 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" t="s">
         <v>271</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
         <v>272</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>274</v>
-      </c>
-      <c r="B4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" t="s">
         <v>276</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
         <v>277</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>278</v>
-      </c>
-      <c r="I5" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B6" t="s">
         <v>368</v>
-      </c>
-      <c r="B6" t="s">
-        <v>369</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -4046,10 +4165,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B7" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -4061,15 +4180,15 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B8" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -4081,15 +4200,15 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>7</v>
@@ -4101,7 +4220,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -4111,10 +4230,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="A27" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4123,16 +4242,16 @@
     <col min="2" max="2" width="102.140625" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="43.5703125" customWidth="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1"/>
+    <col min="8" max="8" width="50.5703125" customWidth="1"/>
     <col min="9" max="9" width="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -4144,24 +4263,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -4173,15 +4292,15 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -4196,18 +4315,18 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -4219,15 +4338,15 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -4244,10 +4363,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -4259,21 +4378,21 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -4285,38 +4404,38 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I9" t="s">
         <v>231</v>
-      </c>
-      <c r="B9" t="s">
-        <v>304</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>282</v>
-      </c>
-      <c r="I9" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -4330,30 +4449,30 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
         <v>234</v>
-      </c>
-      <c r="B11" t="s">
-        <v>306</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -4367,10 +4486,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -4384,10 +4503,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -4401,10 +4520,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -4418,10 +4537,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -4435,10 +4554,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -4452,10 +4571,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -4469,10 +4588,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -4484,15 +4603,15 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -4507,15 +4626,15 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -4527,35 +4646,35 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" t="s">
+        <v>316</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
         <v>258</v>
-      </c>
-      <c r="B22" t="s">
-        <v>317</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -4569,33 +4688,33 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>259</v>
+      </c>
+      <c r="B24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
         <v>260</v>
-      </c>
-      <c r="B24" t="s">
-        <v>318</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>2</v>
-      </c>
-      <c r="I24" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -4607,15 +4726,15 @@
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -4632,10 +4751,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
@@ -4649,10 +4768,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -4669,10 +4788,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -4684,35 +4803,35 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>325</v>
+      </c>
+      <c r="B30" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
         <v>326</v>
-      </c>
-      <c r="B30" t="s">
-        <v>339</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>2</v>
-      </c>
-      <c r="I30" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -4726,30 +4845,30 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>347</v>
+      </c>
+      <c r="B32" t="s">
+        <v>338</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
         <v>348</v>
-      </c>
-      <c r="B32" t="s">
-        <v>339</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" t="s">
-        <v>2</v>
-      </c>
-      <c r="G32" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>349</v>
+      </c>
+      <c r="B33" t="s">
         <v>350</v>
-      </c>
-      <c r="B33" t="s">
-        <v>351</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -4766,10 +4885,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>351</v>
+      </c>
+      <c r="B34" t="s">
         <v>352</v>
-      </c>
-      <c r="B34" t="s">
-        <v>353</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -4783,10 +4902,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>374</v>
+      </c>
+      <c r="B35" t="s">
         <v>375</v>
-      </c>
-      <c r="B35" t="s">
-        <v>376</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -4803,10 +4922,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B36" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -4823,10 +4942,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>377</v>
+      </c>
+      <c r="B37" t="s">
         <v>378</v>
-      </c>
-      <c r="B37" t="s">
-        <v>379</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -4843,10 +4962,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B38" t="s">
-        <v>434</v>
+        <v>513</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -4858,15 +4977,15 @@
         <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B39" t="s">
-        <v>434</v>
+        <v>513</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -4878,15 +4997,15 @@
         <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>434</v>
+        <v>513</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
@@ -4898,15 +5017,15 @@
         <v>2</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>434</v>
+        <v>513</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>7</v>
@@ -4918,75 +5037,75 @@
         <v>2</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>442</v>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -5003,10 +5122,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -5018,15 +5137,15 @@
         <v>2</v>
       </c>
       <c r="I48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -5043,10 +5162,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B50" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -5060,10 +5179,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>341</v>
+      </c>
+      <c r="B51" t="s">
         <v>342</v>
-      </c>
-      <c r="B51" t="s">
-        <v>343</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -5080,10 +5199,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>343</v>
+      </c>
+      <c r="B52" t="s">
         <v>344</v>
-      </c>
-      <c r="B52" t="s">
-        <v>345</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -5097,33 +5216,33 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>345</v>
+      </c>
+      <c r="B53" t="s">
+        <v>342</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
+      <c r="I53" t="s">
         <v>346</v>
-      </c>
-      <c r="B53" t="s">
-        <v>343</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" t="s">
-        <v>2</v>
-      </c>
-      <c r="I53" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>372</v>
+      </c>
+      <c r="B54" t="s">
         <v>373</v>
-      </c>
-      <c r="B54" t="s">
-        <v>374</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -5140,10 +5259,10 @@
     </row>
     <row r="56" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
@@ -5155,15 +5274,15 @@
         <v>2</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>7</v>
@@ -5177,10 +5296,10 @@
     </row>
     <row r="58" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>7</v>
@@ -5192,15 +5311,15 @@
         <v>2</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
@@ -5212,18 +5331,18 @@
         <v>2</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>7</v>
@@ -5235,18 +5354,18 @@
         <v>2</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>7</v>
@@ -5261,10 +5380,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
@@ -5277,15 +5396,15 @@
         <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>7</v>
@@ -5298,12 +5417,76 @@
         <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65" s="8" t="s">
         <v>496</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -5331,10 +5514,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -5346,24 +5529,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
         <v>245</v>
-      </c>
-      <c r="B3" t="s">
-        <v>246</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -5377,30 +5560,30 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s">
         <v>247</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>248</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -5411,11 +5594,11 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" t="s">
         <v>251</v>
       </c>
-      <c r="B6" t="s">
-        <v>252</v>
-      </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -5426,18 +5609,18 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" t="s">
         <v>253</v>
       </c>
-      <c r="B7" t="s">
-        <v>254</v>
-      </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
@@ -5445,10 +5628,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" t="s">
         <v>289</v>
-      </c>
-      <c r="B8" t="s">
-        <v>290</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -5462,10 +5645,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" t="s">
         <v>291</v>
-      </c>
-      <c r="B9" t="s">
-        <v>292</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -5476,10 +5659,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="B10" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -5493,10 +5676,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="B11" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -5510,10 +5693,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="B12" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -5524,10 +5707,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B13" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -5566,10 +5749,10 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -5584,31 +5767,31 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -5617,7 +5800,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -5629,10 +5812,10 @@
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -5644,7 +5827,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" s="1">
         <v>10</v>
@@ -5659,18 +5842,18 @@
         <v>72</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -5682,7 +5865,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -5697,18 +5880,18 @@
         <v>254</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -5720,7 +5903,7 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -5738,18 +5921,18 @@
         <v>4</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -5761,7 +5944,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -5779,18 +5962,18 @@
         <v>5</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -5802,7 +5985,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>

</xml_diff>

<commit_message>
added test that found a bug in function parameters
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="13530"/>
   </bookViews>
   <sheets>
     <sheet name="RegressionTests" sheetId="1" r:id="rId1"/>
@@ -1576,13 +1576,13 @@
     <t>"null transitions not allowed in monitors"; "defer not allowed in monitor"; "monitors cannot have : new | send | monitor | push | pop"; "invalid assignment. right hand side is not a subtype of left hand side"; "Monitors cannot refer to "this"; "invalid payload type in raise"; "invalid payload type in raise (cannot send null value)"; "Monitors cannot be created with "new""; "Undefined machine type"</t>
   </si>
   <si>
-    <t>"invalid assignment. right hand side is not a subtype of left hand side", "insert must be applied to a sequence or a map", "remove must be applied to a sequence or map", "Bad field name", "index must be an integer", "invalid LHS; must have the form LHS ::= var | LHS[expr] | LHS.name", ""in" expects a map", "Value can never be in the map"; "Indexer must be applied to a sequence or map"; ""while (...)" expects a boolean value"; "for insert right syntax is seq += (index value) or map += (key value)"; "value not in the codomain of the map";  "key not in the domain of the map"</t>
-  </si>
-  <si>
     <t>Zinger: assert violation; runtime: valid exe trace</t>
   </si>
   <si>
     <t>This test enables "Unhandled event" exception in Zinger; runtime: valid exe trace</t>
+  </si>
+  <si>
+    <t>"invalid assignment. right hand side is not a subtype of left hand side", "insert must be applied to a sequence or a map", "remove must be applied to a sequence or map", "Bad field name", "index must be an integer", "invalid LHS; must have the form LHS ::= var | LHS[expr] | LHS.name", ""in" expects a map", "Value can never be in the map"; "Indexer must be applied to a sequence or map"; ""while (...)" expects a boolean value"; "for insert right syntax is seq += (index value) or map += (key value)"; "value not in the codomain of the map";  "key not in the domain of the map"; "Index may not be in the domain of the map"</t>
   </si>
 </sst>
 </file>
@@ -1932,7 +1932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
       <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
@@ -3470,7 +3470,7 @@
         <v>418</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4235,7 +4235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
@@ -5443,7 +5443,7 @@
         <v>495</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5463,7 +5463,7 @@
         <v>2</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>497</v>

</xml_diff>

<commit_message>
new cast tests added
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="543">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1646,6 +1646,18 @@
   </si>
   <si>
     <t>4.1.  comparison of "any" type var with "null"</t>
+  </si>
+  <si>
+    <t>CastInExprsDynError3</t>
+  </si>
+  <si>
+    <t>CastInExprsDynError4</t>
+  </si>
+  <si>
+    <t>CastInExprsDynError5</t>
+  </si>
+  <si>
+    <t>CastInExprsDynError6</t>
   </si>
 </sst>
 </file>
@@ -2000,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I173"/>
+  <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4123,26 +4135,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>500</v>
@@ -4157,114 +4152,199 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>516</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B172" t="s">
         <v>519</v>
       </c>
-      <c r="C167" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I167" t="s">
+      <c r="C172" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I172" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>517</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B173" t="s">
         <v>519</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
+      <c r="C173" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B175" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C170" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
+      <c r="C175" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B176" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C171" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
+      <c r="C176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B177" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
+      <c r="C177" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B178" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F173" s="1" t="s">
+      <c r="C178" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F178" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added tests: for short-circuit eval of && and ||; for "-m" option in Zinger
</commit_message>
<xml_diff>
--- a/Doc/TestDocs/Tests.xlsx
+++ b/Doc/TestDocs/Tests.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="551">
   <si>
     <t>Static Error?</t>
   </si>
@@ -1569,9 +1569,6 @@
     <t>"invalid assignment. right hand side is not a subtype of left hand side", "insert must be applied to a sequence or a map", "remove must be applied to a sequence or map", "Bad field name", "index must be an integer", "invalid LHS; must have the form LHS ::= var | LHS[expr] | LHS.name", ""in" expects a map", "Value can never be in the map"; "Indexer must be applied to a sequence or map"; ""while (...)" expects a boolean value"; "for insert right syntax is seq += (index value) or map += (key value)"; "value not in the codomain of the map";  "key not in the domain of the map"; "Index may not be in the domain of the map"</t>
   </si>
   <si>
-    <t>DynamicError\nonAtomicDataTypes16</t>
-  </si>
-  <si>
     <t>BugRepro\PingPongBugRepro.p</t>
   </si>
   <si>
@@ -1657,6 +1654,33 @@
   </si>
   <si>
     <t>Zinger arg: -bc:3</t>
+  </si>
+  <si>
+    <t>SpinlockWithTypestate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinger: "-m" option </t>
+  </si>
+  <si>
+    <t>This is a full version of SLIC Spinlock rule implemented as a P monitor, with test harnesses generated by Zing non-deterministically</t>
+  </si>
+  <si>
+    <t>SpinlockNoTypestate</t>
+  </si>
+  <si>
+    <t>This is a simple version of SLIC Spinlock rule implemented as a regular P machine, with test harnesses generated by Zing non-deterministically</t>
+  </si>
+  <si>
+    <t>Correct\nonAtomicDataTypes16</t>
+  </si>
+  <si>
+    <t>ShortCircuitEval</t>
+  </si>
+  <si>
+    <t>3.5. 3.5. Short-circuit evaluation of “&amp;&amp;” and “||”</t>
+  </si>
+  <si>
+    <t>Tests short-circuit evaluation of “&amp;&amp;” and “||” in Zinger only</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G136" workbookViewId="0">
+      <selection activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3522,7 +3546,7 @@
         <v>353</v>
       </c>
       <c r="I126" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -3530,7 +3554,7 @@
         <v>382</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>2</v>
@@ -3547,7 +3571,7 @@
         <v>383</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>7</v>
@@ -3570,7 +3594,7 @@
         <v>384</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>7</v>
@@ -3593,7 +3617,7 @@
         <v>385</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>7</v>
@@ -3616,7 +3640,7 @@
         <v>386</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>7</v>
@@ -3639,7 +3663,7 @@
         <v>387</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>7</v>
@@ -3662,7 +3686,7 @@
         <v>388</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>7</v>
@@ -3685,7 +3709,7 @@
         <v>397</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>7</v>
@@ -3708,7 +3732,7 @@
         <v>399</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>7</v>
@@ -3731,7 +3755,7 @@
         <v>401</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>7</v>
@@ -3754,7 +3778,7 @@
         <v>403</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>7</v>
@@ -3777,7 +3801,7 @@
         <v>405</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>7</v>
@@ -3800,7 +3824,7 @@
         <v>409</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>7</v>
@@ -3823,7 +3847,7 @@
         <v>414</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>7</v>
@@ -3846,7 +3870,7 @@
         <v>499</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>7</v>
@@ -3869,7 +3893,7 @@
         <v>411</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>7</v>
@@ -3889,28 +3913,28 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>513</v>
+        <v>547</v>
       </c>
       <c r="B146" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G146" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>531</v>
-      </c>
       <c r="H146" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -3918,7 +3942,7 @@
         <v>389</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>7</v>
@@ -3941,7 +3965,7 @@
         <v>501</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>7</v>
@@ -3961,28 +3985,28 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="H149" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -4104,7 +4128,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>498</v>
@@ -4124,7 +4148,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>498</v>
@@ -4141,7 +4165,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>498</v>
@@ -4158,7 +4182,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>498</v>
@@ -4175,7 +4199,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>498</v>
@@ -4192,7 +4216,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>498</v>
@@ -4209,7 +4233,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>498</v>
@@ -4224,12 +4248,35 @@
         <v>2</v>
       </c>
     </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
     <row r="172" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B172" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>7</v>
@@ -4244,15 +4291,15 @@
         <v>2</v>
       </c>
       <c r="I172" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B173" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>7</v>
@@ -4269,10 +4316,10 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>7</v>
@@ -4286,10 +4333,10 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>519</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>7</v>
@@ -4303,10 +4350,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>7</v>
@@ -4320,10 +4367,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>7</v>
@@ -4343,10 +4390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4430,7 +4477,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B5" t="s">
         <v>270</v>
@@ -4445,7 +4492,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4543,6 +4590,46 @@
       </c>
       <c r="I10" s="8" t="s">
         <v>475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>542</v>
+      </c>
+      <c r="B11" t="s">
+        <v>543</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>545</v>
+      </c>
+      <c r="B12" t="s">
+        <v>543</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>